<commit_message>
Recalibrate several transportation variables and update start year
</commit_message>
<xml_diff>
--- a/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
+++ b/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\trans\BAADTbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\trans\BAADTbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,12 +50,12 @@
     <definedName name="ti_tbl_69" localSheetId="3">#REF!</definedName>
     <definedName name="TWh_to_PJ">[1]Notes!$A$15</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="83">
   <si>
     <t>Source:</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Rail</t>
   </si>
   <si>
-    <t>Calculated 2017 Distance Traveled</t>
-  </si>
-  <si>
     <t>Total Passenger Miles</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>See variable SYVbT</t>
+  </si>
+  <si>
+    <t>Calculated 2018 Distance Traveled</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="64">
+  <fills count="65">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1245,6 +1245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2593,7 +2599,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2637,6 +2643,7 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="763">
     <cellStyle name="20% - Accent1 2" xfId="3"/>
@@ -3962,7 +3969,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4022,7 +4029,7 @@
     <row r="10" spans="1:2">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4038,13 +4045,13 @@
     <row r="13" spans="1:2">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4059,7 +4066,7 @@
     <row r="17" spans="1:2">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4068,13 +4075,13 @@
     <row r="19" spans="1:2">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4109,10 +4116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4128,7 +4135,7 @@
     <col min="14" max="14" width="15.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -4147,7 +4154,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -4157,38 +4164,42 @@
       <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="31">
+        <v>2018</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3">
         <v>2007</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>2012</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>2017</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2022</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>2027</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>2032</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>2037</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>2042</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>2047</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>2052</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4196,37 +4207,42 @@
         <v>51</v>
       </c>
       <c r="D4">
+        <f>TREND(H4:I4,H$3:I$3,$D$3)</f>
+        <v>10507.155334034702</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4">
         <v>7285.7384785769091</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>7285.7384785769091</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>9838.9587385820723</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>13179.941715845705</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>16840.937875128242</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>20692.851223700942</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>24299.450439844892</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>27979.322023666995</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>31391.667643013203</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>35418.643120718472</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4234,37 +4250,42 @@
         <v>52</v>
       </c>
       <c r="D5">
+        <f t="shared" ref="D5:D7" si="0">TREND(H5:I5,H$3:I$3,$D$3)</f>
+        <v>10321.245885937009</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5">
         <v>7285.7384785769091</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>7285.7384785769091</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>9694.9739765540417</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>12826.333523469357</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>16183.730543415923</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>19632.973478096745</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>22758.50968024497</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>25863.812309682417</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>28635.326093870575</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>31876.778808646624</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4272,37 +4293,42 @@
         <v>53</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>10135.336437839549</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6">
         <v>7285.7384785769091</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>7285.7384785769091</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>9550.9892145260128</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>12472.72533109301</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>15526.523211703603</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>18573.095732492555</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>21217.568920645052</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>23748.302595697842</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>25878.984544727951</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>28334.914496574776</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4310,72 +4336,82 @@
         <v>54</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>10042.381713790586</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7">
         <v>7285.7384785769091</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>7285.7384785769091</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>9478.9968335119975</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>12295.921234904838</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>15197.919545847442</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>18043.156859690454</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>20447.098540845091</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>22690.547738705551</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>24500.813770156641</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>26563.982340538856</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>55</v>
       </c>
       <c r="D8">
+        <f>TREND(H8:I8,H$3:I$3,$D$3)</f>
+        <v>10507.155334034702</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8">
         <v>7285.7384785769091</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>7285.7384785769091</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>9838.9587385820723</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>13179.941715845705</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>16840.937875128242</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>20692.851223700942</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>24299.450439844892</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>27979.322023666995</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>31391.667643013203</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>35418.643120718472</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -4396,164 +4432,176 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="C12" t="s">
         <v>49</v>
       </c>
       <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="31">
+        <v>2018</v>
+      </c>
+      <c r="G12">
         <v>2007</v>
       </c>
-      <c r="G12">
-        <f>F12+5</f>
+      <c r="H12">
+        <f>G12+5</f>
         <v>2012</v>
       </c>
-      <c r="H12">
-        <f t="shared" ref="H12:O12" si="0">G12+5</f>
+      <c r="I12">
+        <f t="shared" ref="I12:P12" si="1">H12+5</f>
         <v>2017</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
+      <c r="J12">
+        <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
+      <c r="K12">
+        <f t="shared" si="1"/>
         <v>2027</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
+      <c r="L12">
+        <f t="shared" si="1"/>
         <v>2032</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
+      <c r="M12">
+        <f t="shared" si="1"/>
         <v>2037</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
+      <c r="N12">
+        <f t="shared" si="1"/>
         <v>2042</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="0"/>
+      <c r="O12">
+        <f t="shared" si="1"/>
         <v>2047</v>
       </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
+      <c r="P12">
+        <f t="shared" si="1"/>
         <v>2052</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="F13">
-        <f>G13</f>
+      <c r="E13">
+        <f>TREND(I13:J13,I$12:J$12,$E$12)</f>
+        <v>0.84934130751632397</v>
+      </c>
+      <c r="G13">
+        <f>H13</f>
         <v>0.84816017504281249</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.84816017504281249</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.84914445210407208</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.85012872916533166</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.85111300622659114</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.85209728328785073</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.85308156034911031</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>0.85406583741036979</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.85505011447162937</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.85603439153288896</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="D14" t="s">
         <v>22</v>
       </c>
-      <c r="F14">
-        <f t="shared" ref="F14:F15" si="1">G14</f>
+      <c r="E14">
+        <f t="shared" ref="E14:E15" si="2">TREND(I14:J14,I$12:J$12,$E$12)</f>
+        <v>0.14020750072012444</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G15" si="3">H14</f>
         <v>0.14423867048152983</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.14423867048152983</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.14087936234702517</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.13752005421252053</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.13416074607801587</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.13080143794351123</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.12744212980900657</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0.12408282167450192</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>0.12072351353999727</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.11736420540549262</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="D15" t="s">
         <v>23</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>1.0451191763551693E-2</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
         <v>7.6011544756576328E-3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>7.6011544756576328E-3</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>9.9761855489027256E-3</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1.2351216622147818E-2</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1.4726247695392911E-2</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>1.7101278768638005E-2</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1.9476309841883095E-2</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>2.1851340915128189E-2</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>2.4226371988373283E-2</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>2.6601403061618376E-2</v>
       </c>
     </row>
@@ -4586,34 +4634,37 @@
       <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="31">
+        <v>2018</v>
+      </c>
+      <c r="F18">
         <v>2007</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>2012</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>2017</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>2022</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>2027</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>2032</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>2037</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>2042</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>2047</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>2052</v>
       </c>
     </row>
@@ -4628,9 +4679,7 @@
         <v>-1.821267130460829E-2</v>
       </c>
       <c r="D19">
-        <v>0.72850685218433164</v>
-      </c>
-      <c r="E19">
+        <f>TREND(H19:I19,H$18:I$18,$D$18)</f>
         <v>0.72850685218433164</v>
       </c>
       <c r="F19">
@@ -4655,6 +4704,12 @@
         <v>0.72850685218433164</v>
       </c>
       <c r="M19">
+        <v>0.72850685218433164</v>
+      </c>
+      <c r="N19">
+        <v>0.72850685218433164</v>
+      </c>
+      <c r="O19">
         <v>0</v>
       </c>
     </row>
@@ -4666,9 +4721,7 @@
         <v>-3.8954880290412175E-4</v>
       </c>
       <c r="D20">
-        <v>1.5581952116164871E-2</v>
-      </c>
-      <c r="E20">
+        <f t="shared" ref="D20:D24" si="4">TREND(H20:I20,H$18:I$18,$D$18)</f>
         <v>1.5581952116164871E-2</v>
       </c>
       <c r="F20">
@@ -4693,6 +4746,12 @@
         <v>1.5581952116164871E-2</v>
       </c>
       <c r="M20">
+        <v>1.5581952116164871E-2</v>
+      </c>
+      <c r="N20">
+        <v>1.5581952116164871E-2</v>
+      </c>
+      <c r="O20">
         <v>0</v>
       </c>
     </row>
@@ -4704,9 +4763,7 @@
         <v>-1.6956441382425871E-3</v>
       </c>
       <c r="D21">
-        <v>6.7825765529703486E-2</v>
-      </c>
-      <c r="E21">
+        <f t="shared" si="4"/>
         <v>6.7825765529703486E-2</v>
       </c>
       <c r="F21">
@@ -4731,6 +4788,12 @@
         <v>6.7825765529703486E-2</v>
       </c>
       <c r="M21">
+        <v>6.7825765529703486E-2</v>
+      </c>
+      <c r="N21">
+        <v>6.7825765529703486E-2</v>
+      </c>
+      <c r="O21">
         <v>0</v>
       </c>
     </row>
@@ -4742,9 +4805,7 @@
         <v>-3.3728626169377456E-3</v>
       </c>
       <c r="D22">
-        <v>0.13491450467750982</v>
-      </c>
-      <c r="E22">
+        <f t="shared" si="4"/>
         <v>0.13491450467750982</v>
       </c>
       <c r="F22">
@@ -4769,6 +4830,12 @@
         <v>0.13491450467750982</v>
       </c>
       <c r="M22">
+        <v>0.13491450467750982</v>
+      </c>
+      <c r="N22">
+        <v>0.13491450467750982</v>
+      </c>
+      <c r="O22">
         <v>0</v>
       </c>
     </row>
@@ -4780,9 +4847,7 @@
         <v>-8.1955679287822546E-4</v>
       </c>
       <c r="D23">
-        <v>3.278227171512902E-2</v>
-      </c>
-      <c r="E23">
+        <f t="shared" si="4"/>
         <v>3.278227171512902E-2</v>
       </c>
       <c r="F23">
@@ -4807,6 +4872,12 @@
         <v>3.278227171512902E-2</v>
       </c>
       <c r="M23">
+        <v>3.278227171512902E-2</v>
+      </c>
+      <c r="N23">
+        <v>3.278227171512902E-2</v>
+      </c>
+      <c r="O23">
         <v>0</v>
       </c>
     </row>
@@ -4818,9 +4889,7 @@
         <v>-5.0971634442902958E-4</v>
       </c>
       <c r="D24">
-        <v>2.0388653777161182E-2</v>
-      </c>
-      <c r="E24">
+        <f t="shared" si="4"/>
         <v>2.0388653777161182E-2</v>
       </c>
       <c r="F24">
@@ -4845,22 +4914,28 @@
         <v>2.0388653777161182E-2</v>
       </c>
       <c r="M24">
+        <v>2.0388653777161182E-2</v>
+      </c>
+      <c r="N24">
+        <v>2.0388653777161182E-2</v>
+      </c>
+      <c r="O24">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:15" s="28" customFormat="1">
       <c r="B27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -4868,12 +4943,12 @@
         <v>61</v>
       </c>
       <c r="B28">
-        <f>F4*H13*SUM(F21,F24)*10^9*About!$A$25</f>
-        <v>457953387456.98651</v>
+        <f>D4*E13*SUM(D21,D24)*10^9*About!$A$25</f>
+        <v>489167910183.24176</v>
       </c>
       <c r="C28">
         <f>B28/SUM('SYVbT-passenger'!B2:H2)/'AVLo-passengers'!B2</f>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -4881,12 +4956,12 @@
         <v>62</v>
       </c>
       <c r="B29">
-        <f>F4*H13*SUM(F19:F20)*10^9*About!$A$25</f>
-        <v>3862837744392.5889</v>
+        <f>D4*E13*SUM(D19:D20)*10^9*About!$A$25</f>
+        <v>4126132306377.9048</v>
       </c>
       <c r="C29">
         <f>B29/SUM('SYVbT-passenger'!B3:H3)/'AVLo-passengers'!B3</f>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -4894,12 +4969,12 @@
         <v>63</v>
       </c>
       <c r="B30">
-        <f>F4*H15*10^9*About!$A$25</f>
-        <v>60990843236.253647</v>
+        <f>D4*E15*10^9*About!$A$25</f>
+        <v>68234175733.797775</v>
       </c>
       <c r="C30">
         <f>B30/SUM('SYVbT-passenger'!B4:H4)/'AVLo-passengers'!B4</f>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -4907,12 +4982,12 @@
         <v>64</v>
       </c>
       <c r="B31">
-        <f>F4*H14*10^9*About!$A$25</f>
-        <v>861286216260.86877</v>
+        <f>D4*E14*10^9*About!$A$25</f>
+        <v>915392565726.14612</v>
       </c>
       <c r="C31">
         <f>B31/SUM('SYVbT-passenger'!B5:H5)/'AVLo-passengers'!B5</f>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -4920,12 +4995,12 @@
         <v>19</v>
       </c>
       <c r="B32">
-        <f>F4*H13*F22*10^9*About!$A$25</f>
-        <v>700390649506.19861</v>
+        <f>D4*E13*D22*10^9*About!$A$25</f>
+        <v>748129918272.5448</v>
       </c>
       <c r="C32">
         <f>B32/SUM('SYVbT-passenger'!B7:H7)/'AVLo-passengers'!B7</f>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4933,12 +5008,12 @@
         <v>20</v>
       </c>
       <c r="B33">
-        <f>F4*H13*F23*10^9*About!$A$25</f>
-        <v>170184789498.58517</v>
+        <f>D4*E13*D23*10^9*About!$A$25</f>
+        <v>181784740770.8432</v>
       </c>
       <c r="C33">
         <f>B33/SUM('SYVbT-freight'!B7:J7)/'AVLo-freight'!B7</f>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4963,10 +5038,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4978,9 +5053,9 @@
     <col min="8" max="8" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4994,10 +5069,10 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -5007,225 +5082,248 @@
       <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="31">
+        <v>2018</v>
+      </c>
+      <c r="F3">
         <v>2007</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>2012</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>2017</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2022</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>2027</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>2032</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>2037</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>2042</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>2047</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>2052</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4">
+        <f>TREND(H4:I4,H$3:I$3,$D$3)</f>
+        <v>2679.4186686408939</v>
+      </c>
+      <c r="F4">
         <v>1671.7017993824848</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>1671.7017993824848</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>2409.0996388421427</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>3760.6947878361552</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>5663.900438648604</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>8084.1516133946598</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>10529.027370144324</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>12905.090138734526</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>14842.836401151224</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>20270.920907074131</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5">
+        <f t="shared" ref="D5:D8" si="0">TREND(H5:I5,H$3:I$3,$D$3)</f>
+        <v>2631.0352374222712</v>
+      </c>
+      <c r="F5">
         <v>1671.7017993824848</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>1671.7017993824848</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>2373.8445221761599</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>3659.7980984064047</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>5442.8701776281705</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>7670.0853112451769</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>9861.3329515498044</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>11929.339420927769</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>13539.56296105014</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>18243.828816366717</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2606.8435218128143</v>
+      </c>
+      <c r="F6">
         <v>1671.7017993824848</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>1671.7017993824848</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>2356.2169638431687</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>3609.3497536915293</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>5332.3550471179533</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>7463.0521601704349</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>9527.4857422525456</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>11441.46406202439</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>12887.926240999597</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>17230.282771013011</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2582.6518062034738</v>
+      </c>
+      <c r="F7">
         <v>1671.7017993824848</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>1671.7017993824848</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>2338.5894055101776</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>3558.9014089766542</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>5221.8399166077379</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>7256.0190090956949</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>9193.6385329552868</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>10953.588703121011</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>12236.289520949058</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>16216.736725659306</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>55</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2679.4186686408939</v>
+      </c>
+      <c r="F8">
         <v>1671.7017993824848</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>1671.7017993824848</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>2409.0996388421427</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>3760.6947878361552</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>5663.900438648604</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>8084.1516133946598</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>10529.027370144324</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>12905.090138734526</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>14842.836401151224</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>20270.920907074131</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -5235,47 +5333,50 @@
       <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="31">
+        <v>2018</v>
+      </c>
+      <c r="F10">
         <v>2007</v>
       </c>
-      <c r="E10">
-        <f>D10+5</f>
+      <c r="G10">
+        <f>F10+5</f>
         <v>2012</v>
       </c>
-      <c r="F10">
-        <f t="shared" ref="F10:M10" si="0">E10+5</f>
+      <c r="H10">
+        <f t="shared" ref="H10:O10" si="1">G10+5</f>
         <v>2017</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
+      <c r="I10">
+        <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
+      <c r="J10">
+        <f t="shared" si="1"/>
         <v>2027</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
+      <c r="K10">
+        <f t="shared" si="1"/>
         <v>2032</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
+      <c r="L10">
+        <f t="shared" si="1"/>
         <v>2037</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
+      <c r="M10">
+        <f t="shared" si="1"/>
         <v>2042</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
+      <c r="N10">
+        <f t="shared" si="1"/>
         <v>2047</v>
       </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
+      <c r="O10">
+        <f t="shared" si="1"/>
         <v>2052</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5283,109 +5384,121 @@
         <v>13</v>
       </c>
       <c r="D11">
+        <f>TREND(H11:I11,H$10:I$10,$D$10)</f>
+        <v>0.60450760266995829</v>
+      </c>
+      <c r="F11">
         <v>0.58344055099029235</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>0.58344055099029235</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.60099642739001324</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>0.61855230378973403</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>0.63610818018945492</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>0.65366405658917581</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>0.67121993298889671</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>0.6887758093886176</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>0.70633168578833838</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>0.72388756218805927</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="D12">
+        <f t="shared" ref="D12:D13" si="2">TREND(H12:I12,H$10:I$10,$D$10)</f>
+        <v>0.39524003352767334</v>
+      </c>
+      <c r="F12">
         <v>0.41632638436382852</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>0.41632638436382852</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>0.39875442533369859</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>0.38118246630356867</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>0.36361050727343874</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>0.34603854824330882</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>0.32846658921317884</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>0.31089463018304891</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>0.29332267115291899</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>0.27575071212278907</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="D13">
+        <f t="shared" si="2"/>
+        <v>2.5236380237002396E-4</v>
+      </c>
+      <c r="F13">
         <v>2.330646458791455E-4</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>2.330646458791455E-4</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>2.4914727628821135E-4</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>2.6522990669727717E-4</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>2.81312537106343E-4</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>2.9739516751540882E-4</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>3.1347779792447464E-4</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>3.2956042833354052E-4</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>3.4564305874260634E-4</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>3.6172568915167217E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5400,7 +5513,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -5413,6 +5526,9 @@
       <c r="C17" t="s">
         <v>11</v>
       </c>
+      <c r="D17" s="31">
+        <v>2018</v>
+      </c>
       <c r="F17">
         <v>2012</v>
       </c>
@@ -5451,6 +5567,10 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
+      <c r="D18">
+        <f>TREND(G18:H18,G$17:H$17,$D$17)</f>
+        <v>10964986.81390816</v>
+      </c>
       <c r="F18">
         <v>9847950.663638426</v>
       </c>
@@ -5486,6 +5606,10 @@
       <c r="C19" t="s">
         <v>15</v>
       </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D22" si="3">TREND(G19:H19,G$17:H$17,$D$17)</f>
+        <v>1043408.1607697904</v>
+      </c>
       <c r="F19">
         <v>953526.79330709181</v>
       </c>
@@ -5521,6 +5645,10 @@
       <c r="C20" t="s">
         <v>15</v>
       </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>276308695643.09021</v>
+      </c>
       <c r="F20">
         <v>276308695643.09021</v>
       </c>
@@ -5553,6 +5681,10 @@
       <c r="C21" t="s">
         <v>16</v>
       </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>276308695643.09021</v>
+      </c>
       <c r="F21">
         <v>276308695643.09021</v>
       </c>
@@ -5588,6 +5720,10 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>8499909472.5085201</v>
+      </c>
       <c r="F22">
         <v>8499909472.5085201</v>
       </c>
@@ -5618,7 +5754,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="3" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="8"/>
@@ -5626,10 +5762,10 @@
     <row r="25" spans="1:14">
       <c r="A25" s="28"/>
       <c r="B25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -5637,12 +5773,12 @@
         <v>61</v>
       </c>
       <c r="B26">
-        <f>F4*F11*(G19/SUM(G18:G19))*10^9*About!$A$25</f>
-        <v>77839190765.635284</v>
+        <f>D4*D11*(D19/SUM(D18:D19))*10^9*About!$A$25</f>
+        <v>87450559346.503723</v>
       </c>
       <c r="C26">
         <f>IESS_Frgt!B26/SUM('SYVbT-freight'!B2:H2)/'AVLo-freight'!B2</f>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -5650,12 +5786,12 @@
         <v>62</v>
       </c>
       <c r="B27">
-        <f>F4*F11*(G18/SUM(G18:G19))*10^9*About!$A$25</f>
-        <v>821819196898.828</v>
+        <f>D4*D11*(D18/SUM(D18:D19))*10^9*About!$A$25</f>
+        <v>919002041728.20288</v>
       </c>
       <c r="C27">
         <f>B27/SUM('SYVbT-freight'!B3:H3)/'AVLo-freight'!B3</f>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -5663,12 +5799,12 @@
         <v>63</v>
       </c>
       <c r="B28" s="13">
-        <f>F4*F13*10^9*About!A25</f>
-        <v>372959682.72201663</v>
+        <f>D4*D13*10^9*About!A25</f>
+        <v>420163789.81934065</v>
       </c>
       <c r="C28">
         <f>B28/SUM('SYVbT-freight'!B4:H4)/'AVLo-freight'!B4</f>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -5676,23 +5812,23 @@
         <v>64</v>
       </c>
       <c r="B29">
-        <f>F4*F12*10^9*About!A25</f>
-        <v>596913304339.79565</v>
+        <f>D4*D12*10^9*About!A25</f>
+        <v>658040292687.53772</v>
       </c>
       <c r="C29">
         <f>B29/SUM('SYVbT-freight'!B5:H5)/'AVLo-freight'!B5</f>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="8"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="30">
         <v>249210.460885123</v>
@@ -6138,273 +6274,226 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="42.75">
+    <row r="1" spans="1:34" ht="42.75">
       <c r="A1" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="C1" s="4">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D1" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="E1" s="4">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="F1" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G1" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="H1" s="1">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="I1" s="4">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="J1" s="1">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="K1" s="4">
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="L1" s="1">
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="M1" s="4">
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="N1" s="1">
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="O1" s="4">
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="P1" s="1">
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="Q1" s="4">
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="R1" s="1">
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="S1" s="4">
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="T1" s="1">
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="U1" s="4">
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="V1" s="1">
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="W1" s="4">
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="X1" s="1">
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="Y1" s="4">
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="Z1" s="1">
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="AA1" s="4">
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="AB1" s="1">
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="AC1" s="4">
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="AD1" s="1">
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="AE1" s="4">
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="AF1" s="1">
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="AG1" s="4">
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="AH1" s="1">
-        <v>2048</v>
-      </c>
-      <c r="AI1" s="4">
-        <v>2049</v>
-      </c>
-      <c r="AJ1" s="1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:34">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="25">
-        <v>3.7892846421104625</v>
+        <v>2.1633908129876787</v>
       </c>
       <c r="C2" s="25">
-        <f>$B2</f>
-        <v>3.7892846421104625</v>
+        <v>2.1432857584501406</v>
       </c>
       <c r="D2" s="25">
-        <f t="shared" ref="D2:AJ7" si="0">$B2</f>
-        <v>3.7892846421104625</v>
+        <v>2.1231807039126025</v>
       </c>
       <c r="E2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.1052705536531136</v>
       </c>
       <c r="F2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0873604033936246</v>
       </c>
       <c r="G2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0694502531341357</v>
       </c>
       <c r="H2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0515401028746467</v>
       </c>
       <c r="I2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0336299526151578</v>
       </c>
       <c r="J2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.020114123924472</v>
       </c>
       <c r="K2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0065982952337791</v>
       </c>
       <c r="L2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9930824665430862</v>
       </c>
       <c r="M2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9795666378523968</v>
       </c>
       <c r="N2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9660508091617039</v>
       </c>
       <c r="O2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9547955803772439</v>
       </c>
       <c r="P2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9435403515927803</v>
       </c>
       <c r="Q2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9322851228083167</v>
       </c>
       <c r="R2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9210298940238566</v>
       </c>
       <c r="S2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.909774665239393</v>
       </c>
       <c r="T2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9131479041739023</v>
       </c>
       <c r="U2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9165211431084108</v>
       </c>
       <c r="V2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9198943820429202</v>
       </c>
       <c r="W2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9232676209774295</v>
       </c>
       <c r="X2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.926640859911938</v>
       </c>
       <c r="Y2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9390693144039801</v>
       </c>
       <c r="Z2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9514977688960151</v>
       </c>
       <c r="AA2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9639262233880537</v>
       </c>
       <c r="AB2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9763546778800922</v>
       </c>
       <c r="AC2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>1.9887831323721308</v>
       </c>
       <c r="AD2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0144520951104354</v>
       </c>
       <c r="AE2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0401210578487365</v>
       </c>
       <c r="AF2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0657900205870376</v>
       </c>
       <c r="AG2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
+        <v>2.0914589833253387</v>
       </c>
       <c r="AH2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
-      </c>
-      <c r="AI2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
-      </c>
-      <c r="AJ2" s="25">
-        <f t="shared" si="0"/>
-        <v>3.7892846421104625</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36">
+        <v>2.1171279460636399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -6416,139 +6505,131 @@
         <v>45</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="E3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="F3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="G3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="H3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="I3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="J3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="K3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="L3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="P3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="Q3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="R3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="S3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="T3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="U3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="V3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="W3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="X3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="Y3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="Z3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AA3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AB3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AC3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AD3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AE3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AF3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AG3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
       <c r="AH3" s="13">
-        <f t="shared" si="0"/>
+        <f>$B3</f>
         <v>45</v>
       </c>
-      <c r="AI3" s="13">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AJ3" s="13">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36">
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -6556,143 +6637,135 @@
         <v>180</v>
       </c>
       <c r="C4" s="13">
-        <f t="shared" ref="C4:R7" si="1">$B4</f>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="D4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="E4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="F4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="G4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="H4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="I4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="J4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="K4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="L4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="M4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="N4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="O4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="P4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="Q4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="R4" s="13">
-        <f t="shared" si="1"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="S4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="T4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="U4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="V4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="W4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="X4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="Y4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="Z4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AA4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AB4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AC4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AD4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AE4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AF4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AG4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
       <c r="AH4" s="13">
-        <f t="shared" si="0"/>
+        <f>$B4</f>
         <v>180</v>
       </c>
-      <c r="AI4" s="13">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="AJ4" s="13">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36">
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
@@ -6700,143 +6773,135 @@
         <v>1000</v>
       </c>
       <c r="C5" s="13">
-        <f t="shared" si="1"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="D5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="E5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="F5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="H5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="J5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="K5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="L5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="M5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="N5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="O5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="P5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="Q5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="R5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="S5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="T5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="U5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="V5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="W5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="X5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="Y5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="Z5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AA5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AB5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AC5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AD5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AE5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AF5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AG5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
       <c r="AH5" s="13">
-        <f t="shared" si="0"/>
+        <f>$B5</f>
         <v>1000</v>
       </c>
-      <c r="AI5" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="AJ5" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36">
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" s="27" t="s">
         <v>7</v>
       </c>
@@ -6844,143 +6909,135 @@
         <v>756.78378378378375</v>
       </c>
       <c r="C6" s="13">
-        <f t="shared" si="1"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="D6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="E6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="F6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="G6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="H6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="I6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="J6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="K6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="L6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="M6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="N6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="O6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="P6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="Q6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="R6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="S6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="T6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="U6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="V6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="W6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="X6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="Y6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="Z6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AA6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AB6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AC6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AD6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AE6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AF6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AG6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
       <c r="AH6" s="13">
-        <f t="shared" si="0"/>
+        <f>$B6</f>
         <v>756.78378378378375</v>
       </c>
-      <c r="AI6" s="13">
-        <f t="shared" si="0"/>
-        <v>756.78378378378375</v>
-      </c>
-      <c r="AJ6" s="13">
-        <f t="shared" si="0"/>
-        <v>756.78378378378375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36">
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -6988,139 +7045,131 @@
         <v>1.6</v>
       </c>
       <c r="C7" s="25">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="D7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="E7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="F7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="G7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="H7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="I7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="J7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="K7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="L7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="M7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="N7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="O7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="P7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="Q7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="R7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="S7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="T7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="U7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="V7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="W7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="X7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="Y7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="Z7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AA7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AB7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AC7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AD7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AE7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AF7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AG7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
       <c r="AH7" s="25">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="AI7" s="25">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="AJ7" s="25">
-        <f t="shared" si="0"/>
+        <f>$B7</f>
         <v>1.6</v>
       </c>
     </row>
@@ -8130,7 +8179,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -8258,143 +8307,143 @@
       </c>
       <c r="B2" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C28</f>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="C2" s="7">
         <f t="shared" ref="C2:C7" si="0">$B2</f>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:AJ7" si="1">$B2</f>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="R2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="W2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="X2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="Y2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AA2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AC2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AD2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AE2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AG2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AH2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AI2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
       <c r="AJ2" s="7">
         <f t="shared" si="1"/>
-        <v>3999.5613482552903</v>
+        <v>7482.923316436978</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -8403,143 +8452,143 @@
       </c>
       <c r="B3" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C29</f>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="X3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="Y3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="Z3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AA3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AB3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AC3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AD3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AE3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AG3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AH3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AI3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
       <c r="AJ3" s="7">
         <f t="shared" si="1"/>
-        <v>46144.57849954535</v>
+        <v>49289.835273965022</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -8548,143 +8597,143 @@
       </c>
       <c r="B4" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C30</f>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" si="0"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="F4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="P4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="Q4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="R4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="S4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="T4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="U4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="V4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="W4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="X4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="Y4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="Z4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AC4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AD4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AE4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AG4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AH4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AI4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
       <c r="AJ4" s="7">
         <f t="shared" si="1"/>
-        <v>614689.38476185652</v>
+        <v>687690.5003439805</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -8693,143 +8742,143 @@
       </c>
       <c r="B5" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C31</f>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="0"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AE5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AG5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AH5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AI5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
       <c r="AJ5" s="7">
         <f t="shared" si="1"/>
-        <v>135820.27309122137</v>
+        <v>144352.55773899661</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -8983,143 +9032,143 @@
       </c>
       <c r="B7" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C32</f>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AE7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AG7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AH7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AI7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
       <c r="AJ7" s="7">
         <f t="shared" si="1"/>
-        <v>2443.0343538988823</v>
+        <v>2609.553815157286</v>
       </c>
     </row>
   </sheetData>
@@ -9262,143 +9311,143 @@
       </c>
       <c r="B2">
         <f>IESS_Frgt!C26</f>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="C2" s="7">
         <f>$B2</f>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:AJ7" si="0">$B2</f>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="R2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="W2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="X2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="Y2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AA2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AC2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AD2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AE2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AG2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AH2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AI2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
       <c r="AJ2" s="7">
         <f t="shared" si="0"/>
-        <v>15655.225994531987</v>
+        <v>17588.290120330541</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -9407,143 +9456,143 @@
       </c>
       <c r="B3">
         <f>IESS_Frgt!C27</f>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:R7" si="1">$B3</f>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="1"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="X3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="Y3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="Z3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AA3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AB3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AC3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AD3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AE3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AG3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AH3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AI3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
       <c r="AJ3" s="7">
         <f t="shared" si="0"/>
-        <v>23076.357547336804</v>
+        <v>25805.21333850432</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -9552,143 +9601,143 @@
       </c>
       <c r="B4">
         <f>IESS_Frgt!C28</f>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" si="1"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="F4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="P4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="Q4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="R4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="S4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="T4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="U4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="V4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="W4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="X4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="Y4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="Z4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AC4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AD4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AE4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AG4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AH4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AI4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
       <c r="AJ4" s="7">
         <f t="shared" si="0"/>
-        <v>312782.47924195672</v>
+        <v>352370.18357649894</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -9697,143 +9746,143 @@
       </c>
       <c r="B5">
         <f>IESS_Frgt!C29</f>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="1"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AE5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AG5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AH5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AI5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
       <c r="AJ5" s="7">
         <f t="shared" si="0"/>
-        <v>38896.866966203786</v>
+        <v>42880.105933270475</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -9987,143 +10036,143 @@
       </c>
       <c r="B7" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C33</f>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="1"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AE7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AG7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AH7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AI7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
       <c r="AJ7" s="7">
         <f t="shared" si="0"/>
-        <v>11431.534197593695</v>
+        <v>12210.718048570816</v>
       </c>
     </row>
     <row r="12" spans="1:36">

</xml_diff>

<commit_message>
Correct BAADTbVT to use correct SYVbT numbers
</commit_message>
<xml_diff>
--- a/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
+++ b/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\trans\BAADTbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BAADTbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F81F3A-0860-4380-B969-C6CBDA70909B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="18720" windowHeight="6945"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -50,7 +51,18 @@
     <definedName name="ti_tbl_69" localSheetId="3">#REF!</definedName>
     <definedName name="TWh_to_PJ">[1]Notes!$A$15</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -309,7 +321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="17">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -2646,769 +2658,769 @@
     <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="763">
-    <cellStyle name="20% - Accent1 2" xfId="3"/>
-    <cellStyle name="20% - Accent1 2 2" xfId="318"/>
-    <cellStyle name="20% - Accent1 3" xfId="476"/>
-    <cellStyle name="20% - Accent1 4" xfId="480"/>
-    <cellStyle name="20% - Accent1 5" xfId="494"/>
-    <cellStyle name="20% - Accent2 2" xfId="4"/>
-    <cellStyle name="20% - Accent2 2 2" xfId="482"/>
-    <cellStyle name="20% - Accent2 3" xfId="496"/>
-    <cellStyle name="20% - Accent2 4" xfId="457"/>
-    <cellStyle name="20% - Accent3 2" xfId="5"/>
-    <cellStyle name="20% - Accent3 2 2" xfId="484"/>
-    <cellStyle name="20% - Accent3 3" xfId="498"/>
-    <cellStyle name="20% - Accent3 4" xfId="461"/>
-    <cellStyle name="20% - Accent4 2" xfId="6"/>
-    <cellStyle name="20% - Accent4 2 2" xfId="486"/>
-    <cellStyle name="20% - Accent4 3" xfId="500"/>
-    <cellStyle name="20% - Accent4 4" xfId="465"/>
-    <cellStyle name="20% - Accent5 2" xfId="7"/>
-    <cellStyle name="20% - Accent5 2 2" xfId="488"/>
-    <cellStyle name="20% - Accent5 3" xfId="502"/>
-    <cellStyle name="20% - Accent5 4" xfId="469"/>
-    <cellStyle name="20% - Accent6 10" xfId="673"/>
-    <cellStyle name="20% - Accent6 2" xfId="8"/>
-    <cellStyle name="20% - Accent6 2 2" xfId="208"/>
-    <cellStyle name="20% - Accent6 3" xfId="434"/>
-    <cellStyle name="20% - Accent6 3 2" xfId="639"/>
-    <cellStyle name="20% - Accent6 4" xfId="437"/>
-    <cellStyle name="20% - Accent6 4 2" xfId="508"/>
-    <cellStyle name="20% - Accent6 5" xfId="477"/>
-    <cellStyle name="20% - Accent6 6" xfId="490"/>
-    <cellStyle name="20% - Accent6 7" xfId="504"/>
-    <cellStyle name="20% - Accent6 8" xfId="642"/>
-    <cellStyle name="20% - Accent6 9" xfId="661"/>
-    <cellStyle name="20% - Colore 1" xfId="512"/>
-    <cellStyle name="20% - Colore 2" xfId="513"/>
-    <cellStyle name="20% - Colore 3" xfId="514"/>
-    <cellStyle name="20% - Colore 4" xfId="515"/>
-    <cellStyle name="20% - Colore 5" xfId="516"/>
-    <cellStyle name="20% - Colore 6" xfId="517"/>
-    <cellStyle name="40% - Accent1 2" xfId="9"/>
-    <cellStyle name="40% - Accent1 2 2" xfId="481"/>
-    <cellStyle name="40% - Accent1 3" xfId="495"/>
-    <cellStyle name="40% - Accent1 4" xfId="454"/>
-    <cellStyle name="40% - Accent2 2" xfId="10"/>
-    <cellStyle name="40% - Accent2 2 2" xfId="483"/>
-    <cellStyle name="40% - Accent2 3" xfId="497"/>
-    <cellStyle name="40% - Accent2 4" xfId="458"/>
-    <cellStyle name="40% - Accent3 2" xfId="11"/>
-    <cellStyle name="40% - Accent3 2 2" xfId="485"/>
-    <cellStyle name="40% - Accent3 3" xfId="499"/>
-    <cellStyle name="40% - Accent3 4" xfId="462"/>
-    <cellStyle name="40% - Accent4 2" xfId="12"/>
-    <cellStyle name="40% - Accent4 2 2" xfId="487"/>
-    <cellStyle name="40% - Accent4 3" xfId="501"/>
-    <cellStyle name="40% - Accent4 4" xfId="466"/>
-    <cellStyle name="40% - Accent5 2" xfId="13"/>
-    <cellStyle name="40% - Accent5 2 2" xfId="489"/>
-    <cellStyle name="40% - Accent5 3" xfId="503"/>
-    <cellStyle name="40% - Accent5 4" xfId="470"/>
-    <cellStyle name="40% - Accent6 2" xfId="14"/>
-    <cellStyle name="40% - Accent6 2 2" xfId="491"/>
-    <cellStyle name="40% - Accent6 3" xfId="505"/>
-    <cellStyle name="40% - Accent6 4" xfId="472"/>
-    <cellStyle name="40% - Colore 1" xfId="518"/>
-    <cellStyle name="40% - Colore 2" xfId="519"/>
-    <cellStyle name="40% - Colore 3" xfId="520"/>
-    <cellStyle name="40% - Colore 4" xfId="521"/>
-    <cellStyle name="40% - Colore 5" xfId="522"/>
-    <cellStyle name="40% - Colore 6" xfId="523"/>
-    <cellStyle name="60% - Accent1 2" xfId="15"/>
-    <cellStyle name="60% - Accent1 3" xfId="455"/>
-    <cellStyle name="60% - Accent2 2" xfId="16"/>
-    <cellStyle name="60% - Accent2 3" xfId="459"/>
-    <cellStyle name="60% - Accent3 2" xfId="17"/>
-    <cellStyle name="60% - Accent3 3" xfId="463"/>
-    <cellStyle name="60% - Accent4 2" xfId="18"/>
-    <cellStyle name="60% - Accent4 3" xfId="467"/>
-    <cellStyle name="60% - Accent5 2" xfId="19"/>
-    <cellStyle name="60% - Accent5 3" xfId="471"/>
-    <cellStyle name="60% - Accent6 2" xfId="20"/>
-    <cellStyle name="60% - Accent6 3" xfId="473"/>
-    <cellStyle name="60% - Colore 1" xfId="524"/>
-    <cellStyle name="60% - Colore 2" xfId="525"/>
-    <cellStyle name="60% - Colore 3" xfId="526"/>
-    <cellStyle name="60% - Colore 4" xfId="527"/>
-    <cellStyle name="60% - Colore 5" xfId="528"/>
-    <cellStyle name="60% - Colore 6" xfId="529"/>
-    <cellStyle name="A - a heading" xfId="664"/>
-    <cellStyle name="A - bold" xfId="667"/>
-    <cellStyle name="A - bottom border" xfId="669"/>
-    <cellStyle name="A - bottom border 2" xfId="762"/>
-    <cellStyle name="A - header" xfId="666"/>
-    <cellStyle name="A - header 2" xfId="681"/>
-    <cellStyle name="A - header 2 2" xfId="685"/>
-    <cellStyle name="A - normal" xfId="665"/>
-    <cellStyle name="A - percent" xfId="670"/>
-    <cellStyle name="Accent1 2" xfId="21"/>
-    <cellStyle name="Accent1 3" xfId="453"/>
-    <cellStyle name="Accent2 2" xfId="22"/>
-    <cellStyle name="Accent2 3" xfId="456"/>
-    <cellStyle name="Accent3 2" xfId="23"/>
-    <cellStyle name="Accent3 3" xfId="460"/>
-    <cellStyle name="Accent4 2" xfId="24"/>
-    <cellStyle name="Accent4 3" xfId="464"/>
-    <cellStyle name="Accent5 2" xfId="25"/>
-    <cellStyle name="Accent5 3" xfId="468"/>
-    <cellStyle name="Accent6 2" xfId="26"/>
-    <cellStyle name="Accent6 3" xfId="438"/>
-    <cellStyle name="Bad 2" xfId="27"/>
-    <cellStyle name="Bad 3" xfId="444"/>
-    <cellStyle name="Best" xfId="530"/>
-    <cellStyle name="Body: normal cell" xfId="28"/>
-    <cellStyle name="Body: normal cell 2" xfId="29"/>
-    <cellStyle name="BORDERS" xfId="531"/>
-    <cellStyle name="BORDERS 2" xfId="532"/>
-    <cellStyle name="Calc Currency (0)" xfId="533"/>
-    <cellStyle name="Calcolo" xfId="534"/>
-    <cellStyle name="Calcolo 2" xfId="535"/>
-    <cellStyle name="Calcolo 3" xfId="536"/>
-    <cellStyle name="Calculation 2" xfId="30"/>
-    <cellStyle name="Calculation 3" xfId="447"/>
-    <cellStyle name="Cella collegata" xfId="537"/>
-    <cellStyle name="Cella da controllare" xfId="538"/>
-    <cellStyle name="Check Cell 2" xfId="31"/>
-    <cellStyle name="Check Cell 3" xfId="449"/>
-    <cellStyle name="Colore 1" xfId="539"/>
-    <cellStyle name="Colore 2" xfId="540"/>
-    <cellStyle name="Colore 3" xfId="541"/>
-    <cellStyle name="Colore 4" xfId="542"/>
-    <cellStyle name="Colore 5" xfId="543"/>
-    <cellStyle name="Colore 6" xfId="544"/>
-    <cellStyle name="Column - Style5" xfId="545"/>
-    <cellStyle name="Column - Style6" xfId="546"/>
-    <cellStyle name="Column heading" xfId="32"/>
-    <cellStyle name="Column headings" xfId="547"/>
-    <cellStyle name="Column headings 2" xfId="761"/>
-    <cellStyle name="Comma 2" xfId="33"/>
-    <cellStyle name="Comma 2 2" xfId="34"/>
-    <cellStyle name="Comma 2 2 2" xfId="548"/>
-    <cellStyle name="Comma 2 3" xfId="509"/>
-    <cellStyle name="Comma 2 4" xfId="656"/>
-    <cellStyle name="Comma 2 5" xfId="320"/>
-    <cellStyle name="Comma 3" xfId="35"/>
-    <cellStyle name="Comma 3 2" xfId="550"/>
-    <cellStyle name="Comma 3 3" xfId="549"/>
-    <cellStyle name="Comma 3 4" xfId="506"/>
-    <cellStyle name="Comma 4" xfId="36"/>
-    <cellStyle name="Comma 4 2" xfId="645"/>
-    <cellStyle name="Comma 5" xfId="37"/>
-    <cellStyle name="Comma 5 2" xfId="551"/>
-    <cellStyle name="Comma 6" xfId="38"/>
-    <cellStyle name="Comma 7" xfId="39"/>
-    <cellStyle name="Comma 7 2" xfId="662"/>
-    <cellStyle name="Comma 8" xfId="40"/>
-    <cellStyle name="Comma 8 2" xfId="672"/>
-    <cellStyle name="Comma 9" xfId="155"/>
-    <cellStyle name="Comma0" xfId="552"/>
-    <cellStyle name="Copied" xfId="553"/>
-    <cellStyle name="Corner heading" xfId="41"/>
-    <cellStyle name="Currency 2" xfId="42"/>
-    <cellStyle name="Currency 2 2" xfId="640"/>
-    <cellStyle name="Currency 3" xfId="43"/>
-    <cellStyle name="Currency 3 2" xfId="44"/>
-    <cellStyle name="Currency0" xfId="554"/>
-    <cellStyle name="Data" xfId="45"/>
-    <cellStyle name="Data (Number)" xfId="555"/>
-    <cellStyle name="Data (Text)" xfId="556"/>
-    <cellStyle name="Data 2" xfId="46"/>
-    <cellStyle name="Data no deci" xfId="47"/>
-    <cellStyle name="Data Superscript" xfId="48"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="49"/>
-    <cellStyle name="Date" xfId="557"/>
-    <cellStyle name="Entered" xfId="558"/>
-    <cellStyle name="Excel Built-in Normal" xfId="205"/>
-    <cellStyle name="Explanatory Text 2" xfId="50"/>
-    <cellStyle name="Explanatory Text 3" xfId="451"/>
-    <cellStyle name="FIGURES" xfId="559"/>
-    <cellStyle name="Fixed" xfId="560"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="51"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="52"/>
-    <cellStyle name="Footnote Text" xfId="561"/>
-    <cellStyle name="Footnotes: top row" xfId="53"/>
-    <cellStyle name="Footnotes: top row 2" xfId="54"/>
-    <cellStyle name="Good 2" xfId="55"/>
-    <cellStyle name="Good 3" xfId="433"/>
-    <cellStyle name="Grey" xfId="562"/>
-    <cellStyle name="Header: bottom row" xfId="56"/>
-    <cellStyle name="Header: bottom row 2" xfId="57"/>
-    <cellStyle name="Header1" xfId="563"/>
-    <cellStyle name="Header2" xfId="564"/>
-    <cellStyle name="Header2 2" xfId="565"/>
-    <cellStyle name="Header2 3" xfId="566"/>
-    <cellStyle name="Heading 1 2" xfId="58"/>
-    <cellStyle name="Heading 1 3" xfId="440"/>
-    <cellStyle name="Heading 2 2" xfId="59"/>
-    <cellStyle name="Heading 2 3" xfId="441"/>
-    <cellStyle name="Heading 3 2" xfId="60"/>
-    <cellStyle name="Heading 3 3" xfId="442"/>
-    <cellStyle name="Heading 4 2" xfId="61"/>
-    <cellStyle name="Heading 4 3" xfId="443"/>
-    <cellStyle name="Hed Side" xfId="62"/>
-    <cellStyle name="Hed Side 2" xfId="63"/>
-    <cellStyle name="Hed Side bold" xfId="64"/>
-    <cellStyle name="Hed Side Indent" xfId="65"/>
-    <cellStyle name="Hed Side Regular" xfId="66"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="67"/>
-    <cellStyle name="Hed Top" xfId="68"/>
-    <cellStyle name="Hed Top - SECTION" xfId="69"/>
-    <cellStyle name="Hed Top_3-new4" xfId="70"/>
-    <cellStyle name="Hyperlink 10" xfId="216" hidden="1"/>
-    <cellStyle name="Hyperlink 10" xfId="370" hidden="1"/>
-    <cellStyle name="Hyperlink 10" xfId="698"/>
-    <cellStyle name="Hyperlink 100" xfId="306" hidden="1"/>
-    <cellStyle name="Hyperlink 100" xfId="420" hidden="1"/>
-    <cellStyle name="Hyperlink 100" xfId="748"/>
-    <cellStyle name="Hyperlink 101" xfId="307" hidden="1"/>
-    <cellStyle name="Hyperlink 101" xfId="421" hidden="1"/>
-    <cellStyle name="Hyperlink 101" xfId="749"/>
-    <cellStyle name="Hyperlink 102" xfId="308" hidden="1"/>
-    <cellStyle name="Hyperlink 102" xfId="422" hidden="1"/>
-    <cellStyle name="Hyperlink 102" xfId="750"/>
-    <cellStyle name="Hyperlink 103" xfId="309" hidden="1"/>
-    <cellStyle name="Hyperlink 103" xfId="423" hidden="1"/>
-    <cellStyle name="Hyperlink 103" xfId="751"/>
-    <cellStyle name="Hyperlink 104" xfId="310" hidden="1"/>
-    <cellStyle name="Hyperlink 104" xfId="424" hidden="1"/>
-    <cellStyle name="Hyperlink 104" xfId="752"/>
-    <cellStyle name="Hyperlink 105" xfId="311" hidden="1"/>
-    <cellStyle name="Hyperlink 105" xfId="425" hidden="1"/>
-    <cellStyle name="Hyperlink 105" xfId="753"/>
-    <cellStyle name="Hyperlink 106" xfId="312" hidden="1"/>
-    <cellStyle name="Hyperlink 106" xfId="426" hidden="1"/>
-    <cellStyle name="Hyperlink 106" xfId="754"/>
-    <cellStyle name="Hyperlink 107" xfId="313" hidden="1"/>
-    <cellStyle name="Hyperlink 107" xfId="427" hidden="1"/>
-    <cellStyle name="Hyperlink 107" xfId="755"/>
-    <cellStyle name="Hyperlink 108" xfId="314" hidden="1"/>
-    <cellStyle name="Hyperlink 108" xfId="428" hidden="1"/>
-    <cellStyle name="Hyperlink 108" xfId="756"/>
-    <cellStyle name="Hyperlink 109" xfId="315" hidden="1"/>
-    <cellStyle name="Hyperlink 109" xfId="429" hidden="1"/>
-    <cellStyle name="Hyperlink 109" xfId="757"/>
-    <cellStyle name="Hyperlink 11" xfId="217" hidden="1"/>
-    <cellStyle name="Hyperlink 11" xfId="369" hidden="1"/>
-    <cellStyle name="Hyperlink 11" xfId="697"/>
-    <cellStyle name="Hyperlink 110" xfId="316" hidden="1"/>
-    <cellStyle name="Hyperlink 110" xfId="430" hidden="1"/>
-    <cellStyle name="Hyperlink 110" xfId="758"/>
-    <cellStyle name="Hyperlink 111" xfId="317" hidden="1"/>
-    <cellStyle name="Hyperlink 111" xfId="431" hidden="1"/>
-    <cellStyle name="Hyperlink 111" xfId="759"/>
-    <cellStyle name="Hyperlink 112" xfId="638"/>
-    <cellStyle name="Hyperlink 113" xfId="206"/>
-    <cellStyle name="Hyperlink 12" xfId="218" hidden="1"/>
-    <cellStyle name="Hyperlink 12" xfId="368" hidden="1"/>
-    <cellStyle name="Hyperlink 12" xfId="696"/>
-    <cellStyle name="Hyperlink 13" xfId="219" hidden="1"/>
-    <cellStyle name="Hyperlink 13" xfId="367" hidden="1"/>
-    <cellStyle name="Hyperlink 13" xfId="695"/>
-    <cellStyle name="Hyperlink 14" xfId="220" hidden="1"/>
-    <cellStyle name="Hyperlink 14" xfId="366" hidden="1"/>
-    <cellStyle name="Hyperlink 14" xfId="159"/>
-    <cellStyle name="Hyperlink 15" xfId="221" hidden="1"/>
-    <cellStyle name="Hyperlink 15" xfId="365" hidden="1"/>
-    <cellStyle name="Hyperlink 15" xfId="507"/>
-    <cellStyle name="Hyperlink 16" xfId="222" hidden="1"/>
-    <cellStyle name="Hyperlink 16" xfId="364" hidden="1"/>
-    <cellStyle name="Hyperlink 16" xfId="161"/>
-    <cellStyle name="Hyperlink 17" xfId="223" hidden="1"/>
-    <cellStyle name="Hyperlink 17" xfId="363" hidden="1"/>
-    <cellStyle name="Hyperlink 17" xfId="162"/>
-    <cellStyle name="Hyperlink 18" xfId="224" hidden="1"/>
-    <cellStyle name="Hyperlink 18" xfId="362" hidden="1"/>
-    <cellStyle name="Hyperlink 18" xfId="163"/>
-    <cellStyle name="Hyperlink 19" xfId="225" hidden="1"/>
-    <cellStyle name="Hyperlink 19" xfId="361" hidden="1"/>
-    <cellStyle name="Hyperlink 19" xfId="164"/>
-    <cellStyle name="Hyperlink 2" xfId="71"/>
-    <cellStyle name="Hyperlink 2 2" xfId="567"/>
-    <cellStyle name="Hyperlink 2 3" xfId="207" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="319" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="378" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="432" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="204" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="706" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="760"/>
-    <cellStyle name="Hyperlink 20" xfId="226" hidden="1"/>
-    <cellStyle name="Hyperlink 20" xfId="360" hidden="1"/>
-    <cellStyle name="Hyperlink 20" xfId="165"/>
-    <cellStyle name="Hyperlink 21" xfId="227" hidden="1"/>
-    <cellStyle name="Hyperlink 21" xfId="359" hidden="1"/>
-    <cellStyle name="Hyperlink 21" xfId="166"/>
-    <cellStyle name="Hyperlink 22" xfId="228" hidden="1"/>
-    <cellStyle name="Hyperlink 22" xfId="358" hidden="1"/>
-    <cellStyle name="Hyperlink 22" xfId="167"/>
-    <cellStyle name="Hyperlink 23" xfId="229" hidden="1"/>
-    <cellStyle name="Hyperlink 23" xfId="357" hidden="1"/>
-    <cellStyle name="Hyperlink 23" xfId="168"/>
-    <cellStyle name="Hyperlink 24" xfId="230" hidden="1"/>
-    <cellStyle name="Hyperlink 24" xfId="356" hidden="1"/>
-    <cellStyle name="Hyperlink 24" xfId="169"/>
-    <cellStyle name="Hyperlink 25" xfId="231" hidden="1"/>
-    <cellStyle name="Hyperlink 25" xfId="355" hidden="1"/>
-    <cellStyle name="Hyperlink 25" xfId="170"/>
-    <cellStyle name="Hyperlink 26" xfId="232" hidden="1"/>
-    <cellStyle name="Hyperlink 26" xfId="354" hidden="1"/>
-    <cellStyle name="Hyperlink 26" xfId="171"/>
-    <cellStyle name="Hyperlink 27" xfId="233" hidden="1"/>
-    <cellStyle name="Hyperlink 27" xfId="353" hidden="1"/>
-    <cellStyle name="Hyperlink 27" xfId="172"/>
-    <cellStyle name="Hyperlink 28" xfId="234" hidden="1"/>
-    <cellStyle name="Hyperlink 28" xfId="352" hidden="1"/>
-    <cellStyle name="Hyperlink 28" xfId="173"/>
-    <cellStyle name="Hyperlink 29" xfId="235" hidden="1"/>
-    <cellStyle name="Hyperlink 29" xfId="351" hidden="1"/>
-    <cellStyle name="Hyperlink 29" xfId="174"/>
-    <cellStyle name="Hyperlink 3" xfId="209" hidden="1"/>
-    <cellStyle name="Hyperlink 3" xfId="377" hidden="1"/>
-    <cellStyle name="Hyperlink 3" xfId="705"/>
-    <cellStyle name="Hyperlink 30" xfId="236" hidden="1"/>
-    <cellStyle name="Hyperlink 30" xfId="350" hidden="1"/>
-    <cellStyle name="Hyperlink 30" xfId="175"/>
-    <cellStyle name="Hyperlink 31" xfId="237" hidden="1"/>
-    <cellStyle name="Hyperlink 31" xfId="349" hidden="1"/>
-    <cellStyle name="Hyperlink 31" xfId="176"/>
-    <cellStyle name="Hyperlink 32" xfId="238" hidden="1"/>
-    <cellStyle name="Hyperlink 32" xfId="348" hidden="1"/>
-    <cellStyle name="Hyperlink 32" xfId="177"/>
-    <cellStyle name="Hyperlink 33" xfId="239" hidden="1"/>
-    <cellStyle name="Hyperlink 33" xfId="347" hidden="1"/>
-    <cellStyle name="Hyperlink 33" xfId="178"/>
-    <cellStyle name="Hyperlink 34" xfId="240" hidden="1"/>
-    <cellStyle name="Hyperlink 34" xfId="346" hidden="1"/>
-    <cellStyle name="Hyperlink 34" xfId="179"/>
-    <cellStyle name="Hyperlink 35" xfId="241" hidden="1"/>
-    <cellStyle name="Hyperlink 35" xfId="345" hidden="1"/>
-    <cellStyle name="Hyperlink 35" xfId="180"/>
-    <cellStyle name="Hyperlink 36" xfId="242" hidden="1"/>
-    <cellStyle name="Hyperlink 36" xfId="344" hidden="1"/>
-    <cellStyle name="Hyperlink 36" xfId="181"/>
-    <cellStyle name="Hyperlink 37" xfId="243" hidden="1"/>
-    <cellStyle name="Hyperlink 37" xfId="343" hidden="1"/>
-    <cellStyle name="Hyperlink 37" xfId="182"/>
-    <cellStyle name="Hyperlink 38" xfId="244" hidden="1"/>
-    <cellStyle name="Hyperlink 38" xfId="342" hidden="1"/>
-    <cellStyle name="Hyperlink 38" xfId="183"/>
-    <cellStyle name="Hyperlink 39" xfId="245" hidden="1"/>
-    <cellStyle name="Hyperlink 39" xfId="341" hidden="1"/>
-    <cellStyle name="Hyperlink 39" xfId="184"/>
-    <cellStyle name="Hyperlink 4" xfId="210" hidden="1"/>
-    <cellStyle name="Hyperlink 4" xfId="376" hidden="1"/>
-    <cellStyle name="Hyperlink 4" xfId="704"/>
-    <cellStyle name="Hyperlink 40" xfId="246" hidden="1"/>
-    <cellStyle name="Hyperlink 40" xfId="340" hidden="1"/>
-    <cellStyle name="Hyperlink 40" xfId="185"/>
-    <cellStyle name="Hyperlink 41" xfId="247" hidden="1"/>
-    <cellStyle name="Hyperlink 41" xfId="339" hidden="1"/>
-    <cellStyle name="Hyperlink 41" xfId="186"/>
-    <cellStyle name="Hyperlink 42" xfId="248" hidden="1"/>
-    <cellStyle name="Hyperlink 42" xfId="338" hidden="1"/>
-    <cellStyle name="Hyperlink 42" xfId="187"/>
-    <cellStyle name="Hyperlink 43" xfId="249" hidden="1"/>
-    <cellStyle name="Hyperlink 43" xfId="337" hidden="1"/>
-    <cellStyle name="Hyperlink 43" xfId="188"/>
-    <cellStyle name="Hyperlink 44" xfId="250" hidden="1"/>
-    <cellStyle name="Hyperlink 44" xfId="336" hidden="1"/>
-    <cellStyle name="Hyperlink 44" xfId="189"/>
-    <cellStyle name="Hyperlink 45" xfId="251" hidden="1"/>
-    <cellStyle name="Hyperlink 45" xfId="335" hidden="1"/>
-    <cellStyle name="Hyperlink 45" xfId="190"/>
-    <cellStyle name="Hyperlink 46" xfId="252" hidden="1"/>
-    <cellStyle name="Hyperlink 46" xfId="334" hidden="1"/>
-    <cellStyle name="Hyperlink 46" xfId="191"/>
-    <cellStyle name="Hyperlink 47" xfId="253" hidden="1"/>
-    <cellStyle name="Hyperlink 47" xfId="333" hidden="1"/>
-    <cellStyle name="Hyperlink 47" xfId="192"/>
-    <cellStyle name="Hyperlink 48" xfId="254" hidden="1"/>
-    <cellStyle name="Hyperlink 48" xfId="332" hidden="1"/>
-    <cellStyle name="Hyperlink 48" xfId="193"/>
-    <cellStyle name="Hyperlink 49" xfId="255" hidden="1"/>
-    <cellStyle name="Hyperlink 49" xfId="331" hidden="1"/>
-    <cellStyle name="Hyperlink 49" xfId="194"/>
-    <cellStyle name="Hyperlink 5" xfId="211" hidden="1"/>
-    <cellStyle name="Hyperlink 5" xfId="375" hidden="1"/>
-    <cellStyle name="Hyperlink 5" xfId="703"/>
-    <cellStyle name="Hyperlink 50" xfId="256" hidden="1"/>
-    <cellStyle name="Hyperlink 50" xfId="330" hidden="1"/>
-    <cellStyle name="Hyperlink 50" xfId="195"/>
-    <cellStyle name="Hyperlink 51" xfId="257" hidden="1"/>
-    <cellStyle name="Hyperlink 51" xfId="329" hidden="1"/>
-    <cellStyle name="Hyperlink 51" xfId="196"/>
-    <cellStyle name="Hyperlink 52" xfId="258" hidden="1"/>
-    <cellStyle name="Hyperlink 52" xfId="328" hidden="1"/>
-    <cellStyle name="Hyperlink 52" xfId="197"/>
-    <cellStyle name="Hyperlink 53" xfId="259" hidden="1"/>
-    <cellStyle name="Hyperlink 53" xfId="327" hidden="1"/>
-    <cellStyle name="Hyperlink 53" xfId="198"/>
-    <cellStyle name="Hyperlink 54" xfId="260" hidden="1"/>
-    <cellStyle name="Hyperlink 54" xfId="326" hidden="1"/>
-    <cellStyle name="Hyperlink 54" xfId="199"/>
-    <cellStyle name="Hyperlink 55" xfId="261" hidden="1"/>
-    <cellStyle name="Hyperlink 55" xfId="325" hidden="1"/>
-    <cellStyle name="Hyperlink 55" xfId="200"/>
-    <cellStyle name="Hyperlink 56" xfId="262" hidden="1"/>
-    <cellStyle name="Hyperlink 56" xfId="324" hidden="1"/>
-    <cellStyle name="Hyperlink 56" xfId="201"/>
-    <cellStyle name="Hyperlink 57" xfId="263" hidden="1"/>
-    <cellStyle name="Hyperlink 57" xfId="323" hidden="1"/>
-    <cellStyle name="Hyperlink 57" xfId="202"/>
-    <cellStyle name="Hyperlink 58" xfId="264" hidden="1"/>
-    <cellStyle name="Hyperlink 58" xfId="379" hidden="1"/>
-    <cellStyle name="Hyperlink 58" xfId="707"/>
-    <cellStyle name="Hyperlink 59" xfId="265" hidden="1"/>
-    <cellStyle name="Hyperlink 59" xfId="322" hidden="1"/>
-    <cellStyle name="Hyperlink 59" xfId="203"/>
-    <cellStyle name="Hyperlink 6" xfId="212" hidden="1"/>
-    <cellStyle name="Hyperlink 6" xfId="374" hidden="1"/>
-    <cellStyle name="Hyperlink 6" xfId="702"/>
-    <cellStyle name="Hyperlink 60" xfId="266" hidden="1"/>
-    <cellStyle name="Hyperlink 60" xfId="380" hidden="1"/>
-    <cellStyle name="Hyperlink 60" xfId="708"/>
-    <cellStyle name="Hyperlink 61" xfId="267" hidden="1"/>
-    <cellStyle name="Hyperlink 61" xfId="381" hidden="1"/>
-    <cellStyle name="Hyperlink 61" xfId="709"/>
-    <cellStyle name="Hyperlink 62" xfId="268" hidden="1"/>
-    <cellStyle name="Hyperlink 62" xfId="382" hidden="1"/>
-    <cellStyle name="Hyperlink 62" xfId="710"/>
-    <cellStyle name="Hyperlink 63" xfId="269" hidden="1"/>
-    <cellStyle name="Hyperlink 63" xfId="383" hidden="1"/>
-    <cellStyle name="Hyperlink 63" xfId="711"/>
-    <cellStyle name="Hyperlink 64" xfId="270" hidden="1"/>
-    <cellStyle name="Hyperlink 64" xfId="384" hidden="1"/>
-    <cellStyle name="Hyperlink 64" xfId="712"/>
-    <cellStyle name="Hyperlink 65" xfId="271" hidden="1"/>
-    <cellStyle name="Hyperlink 65" xfId="385" hidden="1"/>
-    <cellStyle name="Hyperlink 65" xfId="713"/>
-    <cellStyle name="Hyperlink 66" xfId="272" hidden="1"/>
-    <cellStyle name="Hyperlink 66" xfId="386" hidden="1"/>
-    <cellStyle name="Hyperlink 66" xfId="714"/>
-    <cellStyle name="Hyperlink 67" xfId="273" hidden="1"/>
-    <cellStyle name="Hyperlink 67" xfId="387" hidden="1"/>
-    <cellStyle name="Hyperlink 67" xfId="715"/>
-    <cellStyle name="Hyperlink 68" xfId="274" hidden="1"/>
-    <cellStyle name="Hyperlink 68" xfId="388" hidden="1"/>
-    <cellStyle name="Hyperlink 68" xfId="716"/>
-    <cellStyle name="Hyperlink 69" xfId="275" hidden="1"/>
-    <cellStyle name="Hyperlink 69" xfId="389" hidden="1"/>
-    <cellStyle name="Hyperlink 69" xfId="717"/>
-    <cellStyle name="Hyperlink 7" xfId="213" hidden="1"/>
-    <cellStyle name="Hyperlink 7" xfId="373" hidden="1"/>
-    <cellStyle name="Hyperlink 7" xfId="701"/>
-    <cellStyle name="Hyperlink 70" xfId="276" hidden="1"/>
-    <cellStyle name="Hyperlink 70" xfId="390" hidden="1"/>
-    <cellStyle name="Hyperlink 70" xfId="718"/>
-    <cellStyle name="Hyperlink 71" xfId="277" hidden="1"/>
-    <cellStyle name="Hyperlink 71" xfId="391" hidden="1"/>
-    <cellStyle name="Hyperlink 71" xfId="719"/>
-    <cellStyle name="Hyperlink 72" xfId="278" hidden="1"/>
-    <cellStyle name="Hyperlink 72" xfId="392" hidden="1"/>
-    <cellStyle name="Hyperlink 72" xfId="720"/>
-    <cellStyle name="Hyperlink 73" xfId="279" hidden="1"/>
-    <cellStyle name="Hyperlink 73" xfId="393" hidden="1"/>
-    <cellStyle name="Hyperlink 73" xfId="721"/>
-    <cellStyle name="Hyperlink 74" xfId="280" hidden="1"/>
-    <cellStyle name="Hyperlink 74" xfId="394" hidden="1"/>
-    <cellStyle name="Hyperlink 74" xfId="722"/>
-    <cellStyle name="Hyperlink 75" xfId="281" hidden="1"/>
-    <cellStyle name="Hyperlink 75" xfId="395" hidden="1"/>
-    <cellStyle name="Hyperlink 75" xfId="723"/>
-    <cellStyle name="Hyperlink 76" xfId="282" hidden="1"/>
-    <cellStyle name="Hyperlink 76" xfId="396" hidden="1"/>
-    <cellStyle name="Hyperlink 76" xfId="724"/>
-    <cellStyle name="Hyperlink 77" xfId="283" hidden="1"/>
-    <cellStyle name="Hyperlink 77" xfId="397" hidden="1"/>
-    <cellStyle name="Hyperlink 77" xfId="725"/>
-    <cellStyle name="Hyperlink 78" xfId="284" hidden="1"/>
-    <cellStyle name="Hyperlink 78" xfId="398" hidden="1"/>
-    <cellStyle name="Hyperlink 78" xfId="726"/>
-    <cellStyle name="Hyperlink 79" xfId="285" hidden="1"/>
-    <cellStyle name="Hyperlink 79" xfId="399" hidden="1"/>
-    <cellStyle name="Hyperlink 79" xfId="727"/>
-    <cellStyle name="Hyperlink 8" xfId="214" hidden="1"/>
-    <cellStyle name="Hyperlink 8" xfId="372" hidden="1"/>
-    <cellStyle name="Hyperlink 8" xfId="700"/>
-    <cellStyle name="Hyperlink 80" xfId="286" hidden="1"/>
-    <cellStyle name="Hyperlink 80" xfId="400" hidden="1"/>
-    <cellStyle name="Hyperlink 80" xfId="728"/>
-    <cellStyle name="Hyperlink 81" xfId="287" hidden="1"/>
-    <cellStyle name="Hyperlink 81" xfId="401" hidden="1"/>
-    <cellStyle name="Hyperlink 81" xfId="729"/>
-    <cellStyle name="Hyperlink 82" xfId="288" hidden="1"/>
-    <cellStyle name="Hyperlink 82" xfId="402" hidden="1"/>
-    <cellStyle name="Hyperlink 82" xfId="730"/>
-    <cellStyle name="Hyperlink 83" xfId="289" hidden="1"/>
-    <cellStyle name="Hyperlink 83" xfId="403" hidden="1"/>
-    <cellStyle name="Hyperlink 83" xfId="731"/>
-    <cellStyle name="Hyperlink 84" xfId="290" hidden="1"/>
-    <cellStyle name="Hyperlink 84" xfId="404" hidden="1"/>
-    <cellStyle name="Hyperlink 84" xfId="732"/>
-    <cellStyle name="Hyperlink 85" xfId="291" hidden="1"/>
-    <cellStyle name="Hyperlink 85" xfId="405" hidden="1"/>
-    <cellStyle name="Hyperlink 85" xfId="733"/>
-    <cellStyle name="Hyperlink 86" xfId="292" hidden="1"/>
-    <cellStyle name="Hyperlink 86" xfId="406" hidden="1"/>
-    <cellStyle name="Hyperlink 86" xfId="734"/>
-    <cellStyle name="Hyperlink 87" xfId="293" hidden="1"/>
-    <cellStyle name="Hyperlink 87" xfId="407" hidden="1"/>
-    <cellStyle name="Hyperlink 87" xfId="735"/>
-    <cellStyle name="Hyperlink 88" xfId="294" hidden="1"/>
-    <cellStyle name="Hyperlink 88" xfId="408" hidden="1"/>
-    <cellStyle name="Hyperlink 88" xfId="736"/>
-    <cellStyle name="Hyperlink 89" xfId="295" hidden="1"/>
-    <cellStyle name="Hyperlink 89" xfId="409" hidden="1"/>
-    <cellStyle name="Hyperlink 89" xfId="737"/>
-    <cellStyle name="Hyperlink 9" xfId="215" hidden="1"/>
-    <cellStyle name="Hyperlink 9" xfId="371" hidden="1"/>
-    <cellStyle name="Hyperlink 9" xfId="699"/>
-    <cellStyle name="Hyperlink 90" xfId="296" hidden="1"/>
-    <cellStyle name="Hyperlink 90" xfId="410" hidden="1"/>
-    <cellStyle name="Hyperlink 90" xfId="738"/>
-    <cellStyle name="Hyperlink 91" xfId="297" hidden="1"/>
-    <cellStyle name="Hyperlink 91" xfId="411" hidden="1"/>
-    <cellStyle name="Hyperlink 91" xfId="739"/>
-    <cellStyle name="Hyperlink 92" xfId="298" hidden="1"/>
-    <cellStyle name="Hyperlink 92" xfId="412" hidden="1"/>
-    <cellStyle name="Hyperlink 92" xfId="740"/>
-    <cellStyle name="Hyperlink 93" xfId="299" hidden="1"/>
-    <cellStyle name="Hyperlink 93" xfId="413" hidden="1"/>
-    <cellStyle name="Hyperlink 93" xfId="741"/>
-    <cellStyle name="Hyperlink 94" xfId="300" hidden="1"/>
-    <cellStyle name="Hyperlink 94" xfId="414" hidden="1"/>
-    <cellStyle name="Hyperlink 94" xfId="742"/>
-    <cellStyle name="Hyperlink 95" xfId="301" hidden="1"/>
-    <cellStyle name="Hyperlink 95" xfId="415" hidden="1"/>
-    <cellStyle name="Hyperlink 95" xfId="743"/>
-    <cellStyle name="Hyperlink 96" xfId="302" hidden="1"/>
-    <cellStyle name="Hyperlink 96" xfId="416" hidden="1"/>
-    <cellStyle name="Hyperlink 96" xfId="744"/>
-    <cellStyle name="Hyperlink 97" xfId="303" hidden="1"/>
-    <cellStyle name="Hyperlink 97" xfId="417" hidden="1"/>
-    <cellStyle name="Hyperlink 97" xfId="745"/>
-    <cellStyle name="Hyperlink 98" xfId="304" hidden="1"/>
-    <cellStyle name="Hyperlink 98" xfId="418" hidden="1"/>
-    <cellStyle name="Hyperlink 98" xfId="746"/>
-    <cellStyle name="Hyperlink 99" xfId="305" hidden="1"/>
-    <cellStyle name="Hyperlink 99" xfId="419" hidden="1"/>
-    <cellStyle name="Hyperlink 99" xfId="747"/>
-    <cellStyle name="Input [yellow]" xfId="568"/>
-    <cellStyle name="Input [yellow] 2" xfId="569"/>
-    <cellStyle name="Input [yellow] 3" xfId="570"/>
-    <cellStyle name="Input 2" xfId="72"/>
-    <cellStyle name="Input 3" xfId="156"/>
-    <cellStyle name="Input 4" xfId="657"/>
-    <cellStyle name="ITEMS" xfId="571"/>
-    <cellStyle name="Linked Cell 2" xfId="73"/>
-    <cellStyle name="Linked Cell 3" xfId="448"/>
-    <cellStyle name="m1 - Style1" xfId="572"/>
-    <cellStyle name="MANKAD" xfId="573"/>
-    <cellStyle name="Neutral 2" xfId="74"/>
-    <cellStyle name="Neutral 3" xfId="445"/>
-    <cellStyle name="Neutrale" xfId="574"/>
-    <cellStyle name="no dec" xfId="575"/>
+    <cellStyle name="20% - Accent1 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="318" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent1 3" xfId="476" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent1 4" xfId="480" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent1 5" xfId="494" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="482" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Accent2 3" xfId="496" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent2 4" xfId="457" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - Accent3 2 2" xfId="484" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Accent3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - Accent3 4" xfId="461" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - Accent4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - Accent4 3" xfId="500" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20% - Accent4 4" xfId="465" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="20% - Accent5 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="20% - Accent5 3" xfId="502" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - Accent5 4" xfId="469" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="20% - Accent6 10" xfId="673" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="20% - Accent6 2 2" xfId="208" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="20% - Accent6 3" xfId="434" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="20% - Accent6 3 2" xfId="639" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="20% - Accent6 4" xfId="437" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="20% - Accent6 4 2" xfId="508" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="20% - Accent6 5" xfId="477" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="20% - Accent6 6" xfId="490" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - Accent6 7" xfId="504" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="20% - Accent6 8" xfId="642" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="20% - Accent6 9" xfId="661" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="20% - Colore 1" xfId="512" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="20% - Colore 2" xfId="513" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="20% - Colore 3" xfId="514" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - Colore 4" xfId="515" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="20% - Colore 5" xfId="516" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="20% - Colore 6" xfId="517" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="40% - Accent1 2 2" xfId="481" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="40% - Accent1 3" xfId="495" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="40% - Accent1 4" xfId="454" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="40% - Accent2 2 2" xfId="483" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="40% - Accent2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="40% - Accent2 4" xfId="458" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="40% - Accent3 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="40% - Accent3 3" xfId="499" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="40% - Accent3 4" xfId="462" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="40% - Accent4 2 2" xfId="487" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="40% - Accent4 3" xfId="501" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="40% - Accent4 4" xfId="466" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="40% - Accent5 2 2" xfId="489" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="40% - Accent5 3" xfId="503" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="40% - Accent5 4" xfId="470" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="40% - Accent6 2 2" xfId="491" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="40% - Accent6 3" xfId="505" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="40% - Accent6 4" xfId="472" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="40% - Colore 1" xfId="518" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="40% - Colore 2" xfId="519" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="40% - Colore 3" xfId="520" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="40% - Colore 4" xfId="521" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="40% - Colore 5" xfId="522" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="40% - Colore 6" xfId="523" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="60% - Accent1 3" xfId="455" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="60% - Accent2 3" xfId="459" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="60% - Accent3 3" xfId="463" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="60% - Accent4 3" xfId="467" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="60% - Accent5 3" xfId="471" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="60% - Accent6 3" xfId="473" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="60% - Colore 1" xfId="524" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="60% - Colore 2" xfId="525" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="60% - Colore 3" xfId="526" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="60% - Colore 4" xfId="527" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="60% - Colore 5" xfId="528" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="60% - Colore 6" xfId="529" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="A - a heading" xfId="664" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="A - bold" xfId="667" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="A - bottom border" xfId="669" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="A - bottom border 2" xfId="762" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="A - header" xfId="666" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="A - header 2" xfId="681" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="A - header 2 2" xfId="685" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="A - normal" xfId="665" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="A - percent" xfId="670" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Accent1 3" xfId="453" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Accent2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Accent2 3" xfId="456" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Accent3 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Accent3 3" xfId="460" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Accent4 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Accent4 3" xfId="464" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Accent5 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Accent5 3" xfId="468" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Accent6 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Accent6 3" xfId="438" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Bad 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Bad 3" xfId="444" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Best" xfId="530" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Body: normal cell" xfId="28" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="BORDERS" xfId="531" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="BORDERS 2" xfId="532" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Calc Currency (0)" xfId="533" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Calcolo" xfId="534" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Calcolo 2" xfId="535" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Calcolo 3" xfId="536" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Calculation 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Calculation 3" xfId="447" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Cella collegata" xfId="537" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Cella da controllare" xfId="538" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Check Cell 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Check Cell 3" xfId="449" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Colore 1" xfId="539" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Colore 2" xfId="540" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Colore 3" xfId="541" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Colore 4" xfId="542" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Colore 5" xfId="543" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Colore 6" xfId="544" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Column - Style5" xfId="545" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Column - Style6" xfId="546" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Column heading" xfId="32" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Column headings" xfId="547" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Column headings 2" xfId="761" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Comma 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Comma 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Comma 2 2 2" xfId="548" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Comma 2 3" xfId="509" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Comma 2 4" xfId="656" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Comma 2 5" xfId="320" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Comma 3" xfId="35" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Comma 3 2" xfId="550" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Comma 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Comma 3 4" xfId="506" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Comma 4" xfId="36" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Comma 4 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Comma 5" xfId="37" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Comma 5 2" xfId="551" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Comma 6" xfId="38" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Comma 7" xfId="39" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Comma 7 2" xfId="662" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Comma 8" xfId="40" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Comma 8 2" xfId="672" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Comma 9" xfId="155" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Comma0" xfId="552" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Copied" xfId="553" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Corner heading" xfId="41" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Currency 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Currency 2 2" xfId="640" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Currency 3" xfId="43" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Currency 3 2" xfId="44" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Currency0" xfId="554" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Data" xfId="45" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Data (Number)" xfId="555" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Data (Text)" xfId="556" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Data 2" xfId="46" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Data no deci" xfId="47" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Data Superscript" xfId="48" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="49" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Date" xfId="557" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Entered" xfId="558" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="205" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="50" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Explanatory Text 3" xfId="451" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="FIGURES" xfId="559" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Fixed" xfId="560" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="51" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="52" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Footnote Text" xfId="561" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="53" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="54" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Good 2" xfId="55" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Good 3" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Grey" xfId="562" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Header: bottom row" xfId="56" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="57" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Header1" xfId="563" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Header2" xfId="564" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Header2 2" xfId="565" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Header2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Heading 1 2" xfId="58" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Heading 1 3" xfId="440" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Heading 2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Heading 2 3" xfId="441" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Heading 3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Heading 3 3" xfId="442" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Heading 4 2" xfId="61" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Heading 4 3" xfId="443" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Hed Side" xfId="62" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Hed Side 2" xfId="63" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Hed Side bold" xfId="64" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Hed Side Indent" xfId="65" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="66" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Hed Top" xfId="68" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Hed Top - SECTION" xfId="69" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Hed Top_3-new4" xfId="70" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="216" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="370" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="698" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="306" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="420" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="748" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="307" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="421" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="749" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="308" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="422" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="750" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="309" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="423" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="751" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="310" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="424" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="752" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="311" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="425" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="753" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="312" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="426" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="754" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="313" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="427" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="755" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="314" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="428" hidden="1" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="756" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="315" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="429" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="757" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="217" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="369" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="697" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="316" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="430" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="758" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="317" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="431" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="759" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Hyperlink 112" xfId="638" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Hyperlink 113" xfId="206" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="218" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="368" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="696" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="219" hidden="1" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Hyperlink 13" xfId="367" hidden="1" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Hyperlink 13" xfId="695" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Hyperlink 14" xfId="220" hidden="1" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Hyperlink 14" xfId="366" hidden="1" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Hyperlink 14" xfId="159" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Hyperlink 15" xfId="221" hidden="1" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Hyperlink 15" xfId="365" hidden="1" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Hyperlink 15" xfId="507" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Hyperlink 16" xfId="222" hidden="1" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Hyperlink 16" xfId="364" hidden="1" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Hyperlink 16" xfId="161" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Hyperlink 17" xfId="223" hidden="1" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Hyperlink 17" xfId="363" hidden="1" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Hyperlink 17" xfId="162" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="224" hidden="1" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="362" hidden="1" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="163" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="225" hidden="1" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="361" hidden="1" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="164" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Hyperlink 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="567" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="207" hidden="1" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="319" hidden="1" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="378" hidden="1" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="432" hidden="1" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="204" hidden="1" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="706" hidden="1" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="760" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="226" hidden="1" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="360" hidden="1" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="165" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="227" hidden="1" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="359" hidden="1" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="166" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="228" hidden="1" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="358" hidden="1" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="167" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="229" hidden="1" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="357" hidden="1" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="168" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="230" hidden="1" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="356" hidden="1" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="169" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="231" hidden="1" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="355" hidden="1" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="170" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="232" hidden="1" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="354" hidden="1" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="171" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="233" hidden="1" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="353" hidden="1" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="172" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="234" hidden="1" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="352" hidden="1" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="173" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="235" hidden="1" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="351" hidden="1" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="174" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="209" hidden="1" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="377" hidden="1" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="705" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="236" hidden="1" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="350" hidden="1" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="175" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="237" hidden="1" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="349" hidden="1" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="176" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="238" hidden="1" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="348" hidden="1" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="177" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="239" hidden="1" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="347" hidden="1" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="178" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="240" hidden="1" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="346" hidden="1" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="179" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="241" hidden="1" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="345" hidden="1" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="180" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="242" hidden="1" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="344" hidden="1" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="181" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="243" hidden="1" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="343" hidden="1" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="182" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="244" hidden="1" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="342" hidden="1" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="183" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="245" hidden="1" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="341" hidden="1" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="184" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="210" hidden="1" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="376" hidden="1" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="704" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="246" hidden="1" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="340" hidden="1" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="185" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="247" hidden="1" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="339" hidden="1" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="186" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="248" hidden="1" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="338" hidden="1" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="187" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="249" hidden="1" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="337" hidden="1" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="188" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="250" hidden="1" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="336" hidden="1" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="189" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="251" hidden="1" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="335" hidden="1" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="190" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="252" hidden="1" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="334" hidden="1" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="191" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="253" hidden="1" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="333" hidden="1" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="192" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="254" hidden="1" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="332" hidden="1" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="193" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="255" hidden="1" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="331" hidden="1" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="194" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="211" hidden="1" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="375" hidden="1" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="703" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="256" hidden="1" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="330" hidden="1" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="195" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="257" hidden="1" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="329" hidden="1" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="196" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="258" hidden="1" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="328" hidden="1" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="197" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="259" hidden="1" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="327" hidden="1" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="198" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="260" hidden="1" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="326" hidden="1" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="199" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="261" hidden="1" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="325" hidden="1" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="200" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="262" hidden="1" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="324" hidden="1" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="201" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="263" hidden="1" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="323" hidden="1" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="202" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="264" hidden="1" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="379" hidden="1" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="707" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="265" hidden="1" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="322" hidden="1" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="203" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="212" hidden="1" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="374" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="702" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="266" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="380" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="708" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="267" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="381" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="709" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="268" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="382" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="710" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="269" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="383" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="711" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="270" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="384" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="712" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="271" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="385" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="713" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="272" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="386" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="714" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="273" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="387" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="715" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="274" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="388" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="716" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="275" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="389" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="717" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="213" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="373" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="701" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="276" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="390" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="718" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="277" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="391" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="719" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="278" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="392" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="720" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="279" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="393" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="721" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="280" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="394" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="722" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="281" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="395" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="723" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="282" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="396" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="724" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="283" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="397" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="725" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="284" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="398" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="726" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="285" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="399" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="727" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="214" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="372" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="700" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="286" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="400" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="728" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="287" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="401" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="729" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="288" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="402" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="730" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="289" hidden="1" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="403" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="731" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="290" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="404" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="732" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="291" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="405" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="733" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="292" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="406" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="734" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="293" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="407" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="735" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="294" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="408" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="736" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="295" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="409" hidden="1" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Hyperlink 89" xfId="737" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Hyperlink 9" xfId="215" hidden="1" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Hyperlink 9" xfId="371" hidden="1" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Hyperlink 9" xfId="699" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Hyperlink 90" xfId="296" hidden="1" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Hyperlink 90" xfId="410" hidden="1" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Hyperlink 90" xfId="738" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Hyperlink 91" xfId="297" hidden="1" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Hyperlink 91" xfId="411" hidden="1" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Hyperlink 91" xfId="739" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Hyperlink 92" xfId="298" hidden="1" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Hyperlink 92" xfId="412" hidden="1" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Hyperlink 92" xfId="740" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="299" hidden="1" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="413" hidden="1" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="741" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="300" hidden="1" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="414" hidden="1" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="742" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="301" hidden="1" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="415" hidden="1" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="743" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="302" hidden="1" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="416" hidden="1" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="744" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="303" hidden="1" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="417" hidden="1" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="745" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="304" hidden="1" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="418" hidden="1" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="746" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="305" hidden="1" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="419" hidden="1" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="747" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="Input [yellow]" xfId="568" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="Input [yellow] 2" xfId="569" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="Input [yellow] 3" xfId="570" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Input 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="Input 3" xfId="156" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="Input 4" xfId="657" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="ITEMS" xfId="571" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Linked Cell 2" xfId="73" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Linked Cell 3" xfId="448" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="m1 - Style1" xfId="572" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="MANKAD" xfId="573" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Neutral 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Neutral 3" xfId="445" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Neutrale" xfId="574" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="no dec" xfId="575" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="576"/>
-    <cellStyle name="Normal 10" xfId="75"/>
-    <cellStyle name="Normal 10 2" xfId="577"/>
-    <cellStyle name="Normal 11" xfId="76"/>
-    <cellStyle name="Normal 12" xfId="649"/>
-    <cellStyle name="Normal 13" xfId="655"/>
-    <cellStyle name="Normal 14" xfId="660"/>
-    <cellStyle name="Normal 14 2" xfId="663"/>
-    <cellStyle name="Normal 14 3" xfId="676"/>
-    <cellStyle name="Normal 14 3 2" xfId="683"/>
-    <cellStyle name="Normal 14 3 2 2" xfId="687"/>
-    <cellStyle name="Normal 14 3 2 2 2" xfId="690"/>
-    <cellStyle name="Normal 14 4" xfId="678"/>
-    <cellStyle name="Normal 14 4 2" xfId="680"/>
-    <cellStyle name="Normal 14 4 2 2" xfId="684"/>
-    <cellStyle name="Normal 14 4 2 2 2" xfId="688"/>
-    <cellStyle name="Normal 15" xfId="671"/>
-    <cellStyle name="Normal 16" xfId="692"/>
-    <cellStyle name="Normal 17" xfId="693"/>
-    <cellStyle name="Normal 18" xfId="153"/>
-    <cellStyle name="Normal 19" xfId="659"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="77"/>
-    <cellStyle name="Normal 2 2 2" xfId="436"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="579"/>
-    <cellStyle name="Normal 2 2 3" xfId="580"/>
-    <cellStyle name="Normal 2 2 4" xfId="578"/>
-    <cellStyle name="Normal 2 2 5" xfId="321"/>
-    <cellStyle name="Normal 2 3" xfId="78"/>
-    <cellStyle name="Normal 2 3 2" xfId="581"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 3 2" xfId="79"/>
-    <cellStyle name="Normal 3 2 2" xfId="80"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="81"/>
-    <cellStyle name="Normal 3 2 2 3" xfId="583"/>
-    <cellStyle name="Normal 3 2 3" xfId="82"/>
-    <cellStyle name="Normal 3 2 4" xfId="435"/>
-    <cellStyle name="Normal 3 3" xfId="83"/>
-    <cellStyle name="Normal 3 3 2" xfId="84"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="85"/>
-    <cellStyle name="Normal 3 3 3" xfId="86"/>
-    <cellStyle name="Normal 3 3 4" xfId="584"/>
-    <cellStyle name="Normal 3 4" xfId="87"/>
-    <cellStyle name="Normal 3 4 2" xfId="88"/>
-    <cellStyle name="Normal 3 4 3" xfId="582"/>
-    <cellStyle name="Normal 3 5" xfId="89"/>
-    <cellStyle name="Normal 3 6" xfId="90"/>
-    <cellStyle name="Normal 3 7" xfId="91"/>
-    <cellStyle name="Normal 4" xfId="92"/>
-    <cellStyle name="Normal 4 2" xfId="93"/>
-    <cellStyle name="Normal 4 2 2" xfId="94"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="95"/>
-    <cellStyle name="Normal 4 2 3" xfId="96"/>
-    <cellStyle name="Normal 4 2 4" xfId="586"/>
-    <cellStyle name="Normal 4 3" xfId="97"/>
-    <cellStyle name="Normal 4 3 2" xfId="98"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="99"/>
-    <cellStyle name="Normal 4 3 3" xfId="100"/>
-    <cellStyle name="Normal 4 3 4" xfId="585"/>
-    <cellStyle name="Normal 4 4" xfId="101"/>
-    <cellStyle name="Normal 4 4 2" xfId="102"/>
-    <cellStyle name="Normal 4 5" xfId="103"/>
-    <cellStyle name="Normal 4 6" xfId="104"/>
-    <cellStyle name="Normal 4 7" xfId="105"/>
-    <cellStyle name="Normal 4 8" xfId="474"/>
-    <cellStyle name="Normal 5" xfId="106"/>
-    <cellStyle name="Normal 5 2" xfId="107"/>
-    <cellStyle name="Normal 5 2 2" xfId="587"/>
-    <cellStyle name="Normal 5 3" xfId="108"/>
-    <cellStyle name="Normal 5 4" xfId="478"/>
-    <cellStyle name="Normal 6" xfId="109"/>
-    <cellStyle name="Normal 6 2" xfId="110"/>
-    <cellStyle name="Normal 6 3" xfId="492"/>
-    <cellStyle name="Normal 7" xfId="111"/>
-    <cellStyle name="Normal 7 2" xfId="112"/>
-    <cellStyle name="Normal 7 3" xfId="588"/>
-    <cellStyle name="Normal 7 3 2" xfId="647"/>
-    <cellStyle name="Normal 7 3 2 2" xfId="653"/>
-    <cellStyle name="Normal 8" xfId="113"/>
-    <cellStyle name="Normal 8 2" xfId="590"/>
-    <cellStyle name="Normal 8 2 2" xfId="643"/>
-    <cellStyle name="Normal 8 3" xfId="644"/>
-    <cellStyle name="Normal 8 3 2" xfId="674"/>
-    <cellStyle name="Normal 8 3 2 2" xfId="691"/>
-    <cellStyle name="Normal 8 4" xfId="589"/>
-    <cellStyle name="Normal 9" xfId="114"/>
-    <cellStyle name="Normal 9 2" xfId="641"/>
-    <cellStyle name="Normal 9 3" xfId="648"/>
-    <cellStyle name="Normal 9 4" xfId="651"/>
-    <cellStyle name="Normal 9 5" xfId="652"/>
-    <cellStyle name="Normal 9 6" xfId="654"/>
-    <cellStyle name="Normal 9 6 2" xfId="675"/>
-    <cellStyle name="Normal 9 6 2 2" xfId="694"/>
-    <cellStyle name="Nota" xfId="591"/>
-    <cellStyle name="Nota 2" xfId="592"/>
-    <cellStyle name="Nota 3" xfId="593"/>
-    <cellStyle name="Note 2" xfId="115"/>
-    <cellStyle name="Note 2 2" xfId="116"/>
-    <cellStyle name="Note 2 3" xfId="475"/>
-    <cellStyle name="Note 3" xfId="479"/>
-    <cellStyle name="Note 4" xfId="493"/>
-    <cellStyle name="Num0 - Style7" xfId="594"/>
-    <cellStyle name="Num2 - Style8" xfId="595"/>
-    <cellStyle name="Numeri - Style1" xfId="596"/>
-    <cellStyle name="Numeri - Style1 2" xfId="597"/>
-    <cellStyle name="ofwhich" xfId="157"/>
-    <cellStyle name="Output 2" xfId="117"/>
-    <cellStyle name="Output 3" xfId="446"/>
-    <cellStyle name="Parent row" xfId="118"/>
-    <cellStyle name="Parent row 2" xfId="119"/>
-    <cellStyle name="Percent [2]" xfId="598"/>
-    <cellStyle name="Percent 10" xfId="658"/>
-    <cellStyle name="Percent 2" xfId="120"/>
-    <cellStyle name="Percent 2 2" xfId="121"/>
-    <cellStyle name="Percent 2 2 2" xfId="511"/>
-    <cellStyle name="Percent 2 3" xfId="160"/>
-    <cellStyle name="Percent 3" xfId="122"/>
-    <cellStyle name="Percent 3 2" xfId="123"/>
-    <cellStyle name="Percent 3 3" xfId="599"/>
-    <cellStyle name="Percent 3 4" xfId="646"/>
-    <cellStyle name="Percent 4" xfId="124"/>
-    <cellStyle name="Percent 4 2" xfId="601"/>
-    <cellStyle name="Percent 4 3" xfId="600"/>
-    <cellStyle name="Percent 5" xfId="602"/>
-    <cellStyle name="Percent 6" xfId="510"/>
-    <cellStyle name="Percent 7" xfId="650"/>
-    <cellStyle name="Percent 8" xfId="668"/>
-    <cellStyle name="Percent 8 2" xfId="677"/>
-    <cellStyle name="Percent 8 3" xfId="679"/>
-    <cellStyle name="Percent 8 3 2" xfId="682"/>
-    <cellStyle name="Percent 8 3 2 2" xfId="686"/>
-    <cellStyle name="Percent 8 3 2 2 2" xfId="689"/>
-    <cellStyle name="Percent 9" xfId="154"/>
-    <cellStyle name="Reference" xfId="125"/>
-    <cellStyle name="RevList" xfId="603"/>
-    <cellStyle name="Row heading" xfId="126"/>
-    <cellStyle name="Row headings" xfId="604"/>
-    <cellStyle name="Row headings Level 1" xfId="605"/>
-    <cellStyle name="Row headings Level 2" xfId="606"/>
-    <cellStyle name="Source - Style2" xfId="607"/>
-    <cellStyle name="Source Hed" xfId="127"/>
-    <cellStyle name="Source Letter" xfId="128"/>
-    <cellStyle name="Source Superscript" xfId="129"/>
-    <cellStyle name="Source Superscript 2" xfId="130"/>
-    <cellStyle name="Source Text" xfId="131"/>
-    <cellStyle name="Source Text 2" xfId="132"/>
-    <cellStyle name="Sources list" xfId="608"/>
-    <cellStyle name="Sources list 2" xfId="609"/>
-    <cellStyle name="Sources Title" xfId="610"/>
-    <cellStyle name="Sources Title 2" xfId="611"/>
-    <cellStyle name="State" xfId="133"/>
-    <cellStyle name="style" xfId="612"/>
-    <cellStyle name="style 2" xfId="613"/>
-    <cellStyle name="style 3" xfId="614"/>
-    <cellStyle name="style1" xfId="615"/>
-    <cellStyle name="style2" xfId="616"/>
-    <cellStyle name="Subtotal" xfId="617"/>
-    <cellStyle name="Superscript" xfId="134"/>
-    <cellStyle name="Table  - Style3" xfId="618"/>
-    <cellStyle name="Table  - Style4" xfId="619"/>
-    <cellStyle name="Table  - Style4 2" xfId="620"/>
-    <cellStyle name="Table  - Style6" xfId="621"/>
-    <cellStyle name="Table  - Style6 2" xfId="622"/>
-    <cellStyle name="Table Data" xfId="135"/>
-    <cellStyle name="Table Head Top" xfId="136"/>
-    <cellStyle name="Table Hed Side" xfId="137"/>
-    <cellStyle name="Table no" xfId="623"/>
-    <cellStyle name="Table title" xfId="138"/>
-    <cellStyle name="Table title 2" xfId="139"/>
-    <cellStyle name="Table_HeaderRow" xfId="158"/>
-    <cellStyle name="Testo avviso" xfId="624"/>
-    <cellStyle name="Testo descrittivo" xfId="625"/>
-    <cellStyle name="þ_x001d_ð &amp;ý&amp;†ýG_x0008_ X_x000a__x0007__x0001__x0001_" xfId="626"/>
-    <cellStyle name="þ_x001d_ð&quot;_x000c_Býò_x000c_5ýU_x0001_e_x0005_¹,_x0007__x0001__x0001_" xfId="627"/>
-    <cellStyle name="Title 2" xfId="140"/>
-    <cellStyle name="Title 3" xfId="439"/>
-    <cellStyle name="Title Text" xfId="141"/>
-    <cellStyle name="Title Text 1" xfId="142"/>
-    <cellStyle name="Title Text 2" xfId="143"/>
-    <cellStyle name="Title-1" xfId="144"/>
-    <cellStyle name="Title-2" xfId="145"/>
-    <cellStyle name="Title-3" xfId="146"/>
-    <cellStyle name="Titolo" xfId="628"/>
-    <cellStyle name="Titolo 1" xfId="629"/>
-    <cellStyle name="Titolo 2" xfId="630"/>
-    <cellStyle name="Titolo 3" xfId="631"/>
-    <cellStyle name="Titolo 4" xfId="632"/>
-    <cellStyle name="Total 2" xfId="147"/>
-    <cellStyle name="Total 3" xfId="452"/>
-    <cellStyle name="Totale" xfId="633"/>
-    <cellStyle name="Totale 2" xfId="634"/>
-    <cellStyle name="Totale 3" xfId="635"/>
-    <cellStyle name="Valore non valido" xfId="636"/>
-    <cellStyle name="Valore valido" xfId="637"/>
-    <cellStyle name="Warning Text 2" xfId="148"/>
-    <cellStyle name="Warning Text 3" xfId="450"/>
-    <cellStyle name="Wrap" xfId="149"/>
-    <cellStyle name="Wrap Bold" xfId="150"/>
-    <cellStyle name="Wrap Title" xfId="151"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
+    <cellStyle name="Normal - Style1" xfId="576" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 10" xfId="75" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 10 2" xfId="577" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 11" xfId="76" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 12" xfId="649" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 13" xfId="655" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 14" xfId="660" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 14 2" xfId="663" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 14 3" xfId="676" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 14 3 2" xfId="683" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 14 3 2 2" xfId="687" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 14 3 2 2 2" xfId="690" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 14 4" xfId="678" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 14 4 2" xfId="680" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 14 4 2 2" xfId="684" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 14 4 2 2 2" xfId="688" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 15" xfId="671" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 16" xfId="692" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 17" xfId="693" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 18" xfId="153" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 19" xfId="659" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 2 2" xfId="77" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="436" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="579" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="580" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 2 2 4" xfId="578" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 2 2 5" xfId="321" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 2 3" xfId="78" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 2 3 2" xfId="581" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 3 2" xfId="79" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 3 2 2 3" xfId="583" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="82" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 3 2 4" xfId="435" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="85" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="86" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 3 3 4" xfId="584" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 3 4" xfId="87" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="88" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 3 4 3" xfId="582" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 3 5" xfId="89" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 3 6" xfId="90" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 3 7" xfId="91" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Normal 4" xfId="92" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Normal 4 2" xfId="93" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="96" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Normal 4 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="Normal 4 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="Normal 4 3 2" xfId="98" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Normal 4 3 3" xfId="100" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Normal 4 3 4" xfId="585" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Normal 4 4" xfId="101" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Normal 4 4 2" xfId="102" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Normal 4 5" xfId="103" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Normal 4 6" xfId="104" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Normal 4 7" xfId="105" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="Normal 4 8" xfId="474" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="Normal 5" xfId="106" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="Normal 5 2" xfId="107" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Normal 5 2 2" xfId="587" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Normal 5 3" xfId="108" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Normal 5 4" xfId="478" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Normal 6" xfId="109" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Normal 6 2" xfId="110" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Normal 6 3" xfId="492" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Normal 7" xfId="111" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Normal 7 2" xfId="112" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Normal 7 3" xfId="588" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Normal 7 3 2" xfId="647" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Normal 7 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Normal 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Normal 8 2" xfId="590" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Normal 8 2 2" xfId="643" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Normal 8 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Normal 8 3 2" xfId="674" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Normal 8 3 2 2" xfId="691" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Normal 8 4" xfId="589" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normal 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normal 9 2" xfId="641" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normal 9 3" xfId="648" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normal 9 4" xfId="651" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normal 9 5" xfId="652" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normal 9 6" xfId="654" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 9 6 2" xfId="675" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Normal 9 6 2 2" xfId="694" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Nota" xfId="591" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Nota 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Nota 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Note 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Note 2 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Note 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="Note 3" xfId="479" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="Note 4" xfId="493" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
+    <cellStyle name="Num0 - Style7" xfId="594" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
+    <cellStyle name="Num2 - Style8" xfId="595" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
+    <cellStyle name="Numeri - Style1" xfId="596" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
+    <cellStyle name="Numeri - Style1 2" xfId="597" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
+    <cellStyle name="ofwhich" xfId="157" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
+    <cellStyle name="Output 2" xfId="117" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
+    <cellStyle name="Output 3" xfId="446" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
+    <cellStyle name="Parent row" xfId="118" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
+    <cellStyle name="Parent row 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
+    <cellStyle name="Percent [2]" xfId="598" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
+    <cellStyle name="Percent 10" xfId="658" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
+    <cellStyle name="Percent 2" xfId="120" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
+    <cellStyle name="Percent 2 2" xfId="121" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
+    <cellStyle name="Percent 2 2 2" xfId="511" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
+    <cellStyle name="Percent 2 3" xfId="160" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
+    <cellStyle name="Percent 3" xfId="122" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
+    <cellStyle name="Percent 3 2" xfId="123" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
+    <cellStyle name="Percent 3 3" xfId="599" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
+    <cellStyle name="Percent 3 4" xfId="646" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
+    <cellStyle name="Percent 4" xfId="124" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
+    <cellStyle name="Percent 4 2" xfId="601" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
+    <cellStyle name="Percent 4 3" xfId="600" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
+    <cellStyle name="Percent 5" xfId="602" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
+    <cellStyle name="Percent 6" xfId="510" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
+    <cellStyle name="Percent 7" xfId="650" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
+    <cellStyle name="Percent 8" xfId="668" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
+    <cellStyle name="Percent 8 2" xfId="677" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
+    <cellStyle name="Percent 8 3" xfId="679" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
+    <cellStyle name="Percent 8 3 2" xfId="682" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
+    <cellStyle name="Percent 8 3 2 2" xfId="686" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
+    <cellStyle name="Percent 8 3 2 2 2" xfId="689" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
+    <cellStyle name="Percent 9" xfId="154" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
+    <cellStyle name="Reference" xfId="125" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
+    <cellStyle name="RevList" xfId="603" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
+    <cellStyle name="Row heading" xfId="126" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
+    <cellStyle name="Row headings" xfId="604" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
+    <cellStyle name="Row headings Level 1" xfId="605" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
+    <cellStyle name="Row headings Level 2" xfId="606" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
+    <cellStyle name="Source - Style2" xfId="607" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
+    <cellStyle name="Source Hed" xfId="127" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
+    <cellStyle name="Source Letter" xfId="128" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
+    <cellStyle name="Source Superscript" xfId="129" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
+    <cellStyle name="Source Superscript 2" xfId="130" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
+    <cellStyle name="Source Text" xfId="131" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
+    <cellStyle name="Source Text 2" xfId="132" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
+    <cellStyle name="Sources list" xfId="608" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
+    <cellStyle name="Sources list 2" xfId="609" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
+    <cellStyle name="Sources Title" xfId="610" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
+    <cellStyle name="Sources Title 2" xfId="611" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
+    <cellStyle name="State" xfId="133" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
+    <cellStyle name="style" xfId="612" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
+    <cellStyle name="style 2" xfId="613" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
+    <cellStyle name="style 3" xfId="614" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
+    <cellStyle name="style1" xfId="615" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
+    <cellStyle name="style2" xfId="616" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
+    <cellStyle name="Subtotal" xfId="617" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
+    <cellStyle name="Superscript" xfId="134" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
+    <cellStyle name="Table  - Style3" xfId="618" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
+    <cellStyle name="Table  - Style4" xfId="619" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
+    <cellStyle name="Table  - Style4 2" xfId="620" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
+    <cellStyle name="Table  - Style6" xfId="621" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="Table  - Style6 2" xfId="622" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Table Data" xfId="135" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
+    <cellStyle name="Table Head Top" xfId="136" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
+    <cellStyle name="Table Hed Side" xfId="137" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
+    <cellStyle name="Table no" xfId="623" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
+    <cellStyle name="Table title" xfId="138" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
+    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
+    <cellStyle name="Table_HeaderRow" xfId="158" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
+    <cellStyle name="Testo avviso" xfId="624" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
+    <cellStyle name="Testo descrittivo" xfId="625" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
+    <cellStyle name="þ_x001d_ð &amp;ý&amp;†ýG_x0008_ X_x000a__x0007__x0001__x0001_" xfId="626" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
+    <cellStyle name="þ_x001d_ð&quot;_x000c_Býò_x000c_5ýU_x0001_e_x0005_¹,_x0007__x0001__x0001_" xfId="627" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
+    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-0000E1020000}"/>
+    <cellStyle name="Title 3" xfId="439" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
+    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
+    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
+    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
+    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
+    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
+    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
+    <cellStyle name="Titolo" xfId="628" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
+    <cellStyle name="Titolo 1" xfId="629" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
+    <cellStyle name="Titolo 2" xfId="630" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
+    <cellStyle name="Titolo 3" xfId="631" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
+    <cellStyle name="Titolo 4" xfId="632" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
+    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
+    <cellStyle name="Total 3" xfId="452" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
+    <cellStyle name="Totale" xfId="633" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
+    <cellStyle name="Totale 2" xfId="634" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
+    <cellStyle name="Totale 3" xfId="635" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
+    <cellStyle name="Valore non valido" xfId="636" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
+    <cellStyle name="Valore valido" xfId="637" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
+    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-0000F5020000}"/>
+    <cellStyle name="Warning Text 3" xfId="450" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
+    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
+    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
+    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -3457,13 +3469,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="EnergyCalcTables" pivot="0" count="4">
+    <tableStyle name="EnergyCalcTables" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="3"/>
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="totalRow" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="EnergyCalcTables 2" pivot="0" count="0"/>
+    <tableStyle name="EnergyCalcTables 2" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3755,6 +3767,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3790,6 +3819,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3965,16 +4011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="56.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4107,7 +4153,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="http://nhts.ornl.gov/2009/pub/stt.pdf"/>
+    <hyperlink ref="B7" r:id="rId1" display="http://nhts.ornl.gov/2009/pub/stt.pdf" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -4115,24 +4161,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.265625" customWidth="1"/>
-    <col min="2" max="2" width="25.1328125" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.86328125" customWidth="1"/>
-    <col min="10" max="10" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.86328125" customWidth="1"/>
-    <col min="12" max="12" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -4948,7 +4994,7 @@
       </c>
       <c r="C28">
         <f>B28/SUM('SYVbT-passenger'!B2:H2)/'AVLo-passengers'!B2</f>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -4961,7 +5007,7 @@
       </c>
       <c r="C29">
         <f>B29/SUM('SYVbT-passenger'!B3:H3)/'AVLo-passengers'!B3</f>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -5000,7 +5046,7 @@
       </c>
       <c r="C32">
         <f>B32/SUM('SYVbT-passenger'!B7:H7)/'AVLo-passengers'!B7</f>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -5013,7 +5059,7 @@
       </c>
       <c r="C33">
         <f>B33/SUM('SYVbT-freight'!B7:J7)/'AVLo-freight'!B7</f>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -5037,20 +5083,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.3984375" customWidth="1"/>
-    <col min="2" max="3" width="21.19921875" customWidth="1"/>
-    <col min="5" max="5" width="13.265625" customWidth="1"/>
-    <col min="6" max="6" width="22.86328125" customWidth="1"/>
-    <col min="8" max="8" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -5778,7 +5824,7 @@
       </c>
       <c r="C26">
         <f>IESS_Frgt!B26/SUM('SYVbT-freight'!B2:H2)/'AVLo-freight'!B2</f>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -5791,7 +5837,7 @@
       </c>
       <c r="C27">
         <f>B27/SUM('SYVbT-freight'!B3:H3)/'AVLo-freight'!B3</f>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -5840,26 +5886,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" customWidth="1"/>
-    <col min="3" max="3" width="20.86328125" customWidth="1"/>
-    <col min="4" max="4" width="18.265625" customWidth="1"/>
-    <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" customWidth="1"/>
-    <col min="7" max="7" width="19.265625" customWidth="1"/>
-    <col min="8" max="8" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="14" t="s">
         <v>37</v>
       </c>
@@ -5890,22 +5936,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="13">
-        <v>572938.26338489645</v>
+        <v>615848.20150874218</v>
       </c>
       <c r="C2" s="13">
-        <v>790583.76150377747</v>
+        <v>849794.15546040237</v>
       </c>
       <c r="D2" s="13">
-        <v>21349037.231082339</v>
+        <v>22947963.197690364</v>
       </c>
       <c r="E2" s="13">
-        <v>6713880.5592320785</v>
+        <v>7216713.4432944935</v>
       </c>
       <c r="F2" s="13">
         <v>0</v>
       </c>
       <c r="G2" s="13">
-        <v>790583.76150377747</v>
+        <v>849794.15546040237</v>
       </c>
       <c r="H2" s="13">
         <v>0</v>
@@ -5916,16 +5962,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="13">
-        <v>7963.3597125818605</v>
+        <v>8406.8117715651661</v>
       </c>
       <c r="C3" s="13">
-        <v>25264.04963461517</v>
+        <v>26670.917493544803</v>
       </c>
       <c r="D3" s="13">
         <v>0</v>
       </c>
       <c r="E3" s="13">
-        <v>1827030.9688959918</v>
+        <v>1928772.0272212988</v>
       </c>
       <c r="F3" s="13">
         <v>0</v>
@@ -6020,13 +6066,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="23">
-        <v>7084729.7365051452</v>
+        <v>7487182.6612117002</v>
       </c>
       <c r="C7" s="23">
         <v>0</v>
       </c>
       <c r="D7" s="23">
-        <v>172095786.18328547</v>
+        <v>181871805.17837322</v>
       </c>
       <c r="E7" s="23">
         <v>0</v>
@@ -6065,26 +6111,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J7"/>
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" customWidth="1"/>
-    <col min="3" max="3" width="20.86328125" customWidth="1"/>
-    <col min="4" max="4" width="18.265625" customWidth="1"/>
-    <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" customWidth="1"/>
-    <col min="7" max="7" width="15.73046875" customWidth="1"/>
-    <col min="8" max="8" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="14" t="s">
         <v>37</v>
       </c>
@@ -6125,7 +6171,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="10">
-        <v>2924758.7540349611</v>
+        <v>3091878.5080698477</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
@@ -6151,7 +6197,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="10">
-        <v>5838202.9413282741</v>
+        <v>6177534.8826565482</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
@@ -6246,22 +6292,22 @@
         <v>8</v>
       </c>
       <c r="B7" s="23">
-        <v>285481.08014483069</v>
+        <v>293883.87403966149</v>
       </c>
       <c r="C7" s="23">
-        <v>956418.05455054785</v>
+        <v>984569.07522626547</v>
       </c>
       <c r="D7" s="23">
-        <v>3383479.4683831781</v>
+        <v>3483068.1367663583</v>
       </c>
       <c r="E7" s="23">
-        <v>3100387.1896618223</v>
+        <v>3191643.3756608572</v>
       </c>
       <c r="F7" s="23">
         <v>0</v>
       </c>
       <c r="G7" s="23">
-        <v>732932.87821756757</v>
+        <v>754505.88022275455</v>
       </c>
       <c r="H7" s="23">
         <v>0</v>
@@ -6273,19 +6319,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="42.75">
+    <row r="1" spans="1:34" ht="45">
       <c r="A1" s="14" t="s">
         <v>45</v>
       </c>
@@ -6501,131 +6547,131 @@
         <v>45</v>
       </c>
       <c r="C3" s="13">
-        <f>$B3</f>
+        <f t="shared" ref="C3:L7" si="0">$B3</f>
         <v>45</v>
       </c>
       <c r="D3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="E3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="F3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="G3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="H3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="I3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="J3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="K3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="L3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="M3" s="13">
-        <f>$B3</f>
+        <f t="shared" ref="M3:V7" si="1">$B3</f>
         <v>45</v>
       </c>
       <c r="N3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="O3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="P3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="Q3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="R3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="S3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="T3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="U3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="V3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="W3" s="13">
-        <f>$B3</f>
+        <f t="shared" ref="W3:AH7" si="2">$B3</f>
         <v>45</v>
       </c>
       <c r="X3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Z3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AA3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AB3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AC3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AD3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AE3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AF3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AG3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AH3" s="13">
-        <f>$B3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
     </row>
@@ -6637,131 +6683,131 @@
         <v>180</v>
       </c>
       <c r="C4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="D4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="E4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="F4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="G4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="H4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="I4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="J4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="K4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="L4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="M4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="N4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="O4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="P4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="Q4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="R4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="S4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="T4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="U4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="V4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="W4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="X4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="Y4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="Z4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AA4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AB4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AC4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AD4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AE4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AF4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AG4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AH4" s="13">
-        <f>$B4</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
     </row>
@@ -6773,131 +6819,131 @@
         <v>1000</v>
       </c>
       <c r="C5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="D5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="G5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="H5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="I5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="J5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="K5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="L5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="M5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="N5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="O5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="P5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="Q5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="R5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="S5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="T5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="U5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="V5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="W5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="X5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="Y5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="Z5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AA5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AB5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AC5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AD5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AE5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AF5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AG5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="AH5" s="13">
-        <f>$B5</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
     </row>
@@ -6909,131 +6955,131 @@
         <v>756.78378378378375</v>
       </c>
       <c r="C6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="D6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="E6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="F6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="G6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="H6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="I6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="J6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="K6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="L6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>756.78378378378375</v>
       </c>
       <c r="M6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="N6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="O6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="P6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="Q6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="R6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="S6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="T6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="U6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="V6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>756.78378378378375</v>
       </c>
       <c r="W6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="X6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="Y6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="Z6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AA6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AB6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AC6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AD6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AE6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AF6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AG6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
       <c r="AH6" s="13">
-        <f>$B6</f>
+        <f t="shared" si="2"/>
         <v>756.78378378378375</v>
       </c>
     </row>
@@ -7042,135 +7088,135 @@
         <v>8</v>
       </c>
       <c r="B7" s="25">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="C7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="G7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="H7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="J7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="K7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="N7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="O7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="P7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="Q7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="R7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="S7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="T7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="U7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="W7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="X7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="Y7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="Z7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AA7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AB7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AC7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AD7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AE7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AF7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AG7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AH7" s="25">
-        <f>$B7</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7179,19 +7225,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="42.75">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="45">
       <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
@@ -8026,143 +8072,143 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="T7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="U7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="V7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="W7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="Y7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="Z7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AA7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AB7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AC7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AD7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AE7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AF7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AG7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AI7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8172,7 +8218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8182,13 +8228,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" style="6" customWidth="1"/>
-    <col min="4" max="36" width="9.59765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.1328125" style="6"/>
+    <col min="1" max="1" width="16.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="6" customWidth="1"/>
+    <col min="4" max="36" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -8307,143 +8353,143 @@
       </c>
       <c r="B2" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C28</f>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="C2" s="7">
         <f t="shared" ref="C2:C7" si="0">$B2</f>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:AJ7" si="1">$B2</f>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="R2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="W2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="X2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="Y2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AA2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AC2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AD2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AE2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AG2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AH2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AI2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
       <c r="AJ2" s="7">
         <f t="shared" si="1"/>
-        <v>7482.923316436978</v>
+        <v>6961.5419505303107</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -8452,143 +8498,143 @@
       </c>
       <c r="B3" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C29</f>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="X3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="Y3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="Z3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AA3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AB3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AC3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AD3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AE3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AG3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AH3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AI3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
       <c r="AJ3" s="7">
         <f t="shared" si="1"/>
-        <v>49289.835273965022</v>
+        <v>46689.839040777297</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -9032,143 +9078,143 @@
       </c>
       <c r="B7" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C32</f>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AE7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AG7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AH7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AI7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
       <c r="AJ7" s="7">
         <f t="shared" si="1"/>
-        <v>2609.553815157286</v>
+        <v>1975.4275379479784</v>
       </c>
     </row>
   </sheetData>
@@ -9178,7 +9224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9188,11 +9234,11 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="9" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="6"/>
+    <col min="3" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -9311,143 +9357,143 @@
       </c>
       <c r="B2">
         <f>IESS_Frgt!C26</f>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="C2" s="7">
         <f>$B2</f>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:AJ7" si="0">$B2</f>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="R2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="W2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="X2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="Y2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AA2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AC2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AD2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AE2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AG2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AH2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AI2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
       <c r="AJ2" s="7">
         <f t="shared" si="0"/>
-        <v>17588.290120330541</v>
+        <v>16637.621874106728</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -9456,143 +9502,143 @@
       </c>
       <c r="B3">
         <f>IESS_Frgt!C27</f>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:R7" si="1">$B3</f>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="1"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="X3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="Y3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="Z3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AA3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AB3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AC3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AD3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AE3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AG3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AH3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AI3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
       <c r="AJ3" s="7">
         <f t="shared" si="0"/>
-        <v>25805.21333850432</v>
+        <v>24387.733177748134</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -10036,143 +10082,143 @@
       </c>
       <c r="B7" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C33</f>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="1"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AE7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AG7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AH7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AI7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
       <c r="AJ7" s="7">
         <f t="shared" si="0"/>
-        <v>12210.718048570816</v>
+        <v>10438.196075004727</v>
       </c>
     </row>
     <row r="12" spans="1:36">

</xml_diff>

<commit_message>
Updated input data from WRI
</commit_message>
<xml_diff>
--- a/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
+++ b/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BAADTbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3D0AE4-0F8C-4736-A0CB-A769679F33CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6C28241-CFD1-444E-B3E1-5EEF3AC074A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -5491,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5642,7 +5642,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6469,7 +6469,7 @@
       </c>
       <c r="C29">
         <f>B29/SUM('SYVbT-passenger'!B3:H3)/'AVLo-passengers'!B3</f>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -6508,7 +6508,7 @@
       </c>
       <c r="C32">
         <f>B32/SUM('SYVbT-passenger'!B7:H7)/'AVLo-passengers'!B7</f>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -6521,7 +6521,7 @@
       </c>
       <c r="C33">
         <f>B33/SUM('SYVbT-freight'!B7:J7)/'AVLo-freight'!B7</f>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -7352,7 +7352,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7401,19 +7401,19 @@
         <v>615848.20150874218</v>
       </c>
       <c r="C2" s="13">
-        <v>849794.15546040249</v>
+        <v>849794.15546040237</v>
       </c>
       <c r="D2" s="13">
-        <v>22947963.197690368</v>
+        <v>22947963.197690364</v>
       </c>
       <c r="E2" s="13">
-        <v>7216713.4432944926</v>
+        <v>7216713.4432944935</v>
       </c>
       <c r="F2" s="13">
         <v>0</v>
       </c>
       <c r="G2" s="13">
-        <v>849794.15546040249</v>
+        <v>849794.15546040237</v>
       </c>
       <c r="H2" s="13">
         <v>0</v>
@@ -7424,16 +7424,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="13">
-        <v>8406.8117715651679</v>
+        <v>8406.8117715651661</v>
       </c>
       <c r="C3" s="13">
-        <v>26670.91749354481</v>
+        <v>26670.917493544803</v>
       </c>
       <c r="D3" s="13">
         <v>0</v>
       </c>
       <c r="E3" s="13">
-        <v>1928772.027221299</v>
+        <v>1928772.0272212988</v>
       </c>
       <c r="F3" s="13">
         <v>0</v>
@@ -7476,7 +7476,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="23">
-        <v>3240.4386067881537</v>
+        <v>3240.4386067881528</v>
       </c>
       <c r="C5" s="23">
         <v>0</v>
@@ -7485,7 +7485,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="23">
-        <v>3100.928529783575</v>
+        <v>3100.9285297835759</v>
       </c>
       <c r="F5" s="23">
         <v>0</v>
@@ -7528,7 +7528,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="23">
-        <v>7487182.6612117011</v>
+        <v>7487182.6612117002</v>
       </c>
       <c r="C7" s="23">
         <v>0</v>
@@ -7577,7 +7577,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7711,7 +7711,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="23">
-        <v>1793.083933506947</v>
+        <v>1793.0839335069468</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -7754,22 +7754,22 @@
         <v>8</v>
       </c>
       <c r="B7" s="23">
-        <v>293883.8740396616</v>
+        <v>293883.87403966149</v>
       </c>
       <c r="C7" s="23">
-        <v>984569.0752262657</v>
+        <v>984569.07522626547</v>
       </c>
       <c r="D7" s="23">
-        <v>3483068.1367663592</v>
+        <v>3483068.1367663583</v>
       </c>
       <c r="E7" s="23">
-        <v>3191643.3756608581</v>
+        <v>3191643.3756608572</v>
       </c>
       <c r="F7" s="23">
         <v>0</v>
       </c>
       <c r="G7" s="23">
-        <v>754505.88022275467</v>
+        <v>754505.88022275455</v>
       </c>
       <c r="H7" s="23">
         <v>0</v>
@@ -7785,7 +7785,7 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AH7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8550,103 +8550,135 @@
         <v>8</v>
       </c>
       <c r="B7" s="25">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="C7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="D7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="E7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="F7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="G7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="H7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="I7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="J7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="K7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="L7" s="25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
       </c>
       <c r="M7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="N7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="O7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="P7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="Q7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="R7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="S7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="T7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="U7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="V7" s="25">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="W7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="X7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="Y7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="Z7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AA7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AB7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AC7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AD7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AE7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AF7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AG7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="AH7" s="25">
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
     </row>
   </sheetData>
@@ -8659,7 +8691,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9502,111 +9534,143 @@
         <v>8</v>
       </c>
       <c r="B7" s="10">
-        <v>2</v>
+        <v>1.76</v>
       </c>
       <c r="C7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="D7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="E7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="F7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="G7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="H7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="I7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="J7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="K7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="L7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="M7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="N7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="O7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="P7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="Q7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="R7" s="10">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
       </c>
       <c r="S7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="T7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="U7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="V7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="W7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="X7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="Y7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="Z7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AA7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AB7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AC7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AD7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AE7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AF7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AG7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AH7" s="10">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="AI7" s="10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.76</v>
       </c>
       <c r="AJ7" s="10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.76</v>
       </c>
     </row>
   </sheetData>
@@ -9623,7 +9687,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9896,143 +9960,143 @@
       </c>
       <c r="B3" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C29</f>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="X3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="Y3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="Z3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AA3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AB3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AC3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AD3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AE3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AG3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AH3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AI3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
       <c r="AJ3" s="7">
         <f t="shared" si="1"/>
-        <v>41202.815141595776</v>
+        <v>41202.815141595784</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -10476,143 +10540,143 @@
       </c>
       <c r="B7" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C32</f>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AE7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AG7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AH7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AI7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
       <c r="AJ7" s="7">
         <f t="shared" si="1"/>
-        <v>1862.9790080705416</v>
+        <v>2328.7237600881767</v>
       </c>
     </row>
   </sheetData>
@@ -10629,7 +10693,7 @@
   <dimension ref="A1:AJ24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11480,143 +11544,143 @@
       </c>
       <c r="B7" s="7">
         <f>IESS_Psng_ROAD_RAIL_AIR!C33</f>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="1"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AE7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AG7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AH7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AI7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
       <c r="AJ7" s="7">
         <f t="shared" si="0"/>
-        <v>13114.951906058117</v>
+        <v>14903.354438702409</v>
       </c>
     </row>
     <row r="12" spans="1:36">
@@ -11743,15 +11807,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D1F9699F1D82E8489539652D1D3605E0" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9beb7d2dcc3a763e4f6e08e0afcdcee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0f2b0006-c2ac-4c37-974f-93953e9e2787" xmlns:ns3="f1a64cc1-e1f5-4dc9-b425-36e48be156d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9081579eb20b52d63b9dedce7867af6d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -12005,7 +12060,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -12014,15 +12069,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1577F24-7C19-4452-8C87-A0EC63571135}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB53E47F-60A7-41CE-A74E-44C5ADB5C133}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12042,12 +12098,28 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF2AE969-1C05-46BB-A2EC-41027AF75ABB}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f1a64cc1-e1f5-4dc9-b425-36e48be156d1"/>
+    <ds:schemaRef ds:uri="0f2b0006-c2ac-4c37-974f-93953e9e2787"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1577F24-7C19-4452-8C87-A0EC63571135}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>